<commit_message>
replaced na with NA
</commit_message>
<xml_diff>
--- a/WarkentinJungRuedaMcDaniel-DataForDeposit.xlsx
+++ b/WarkentinJungRuedaMcDaniel-DataForDeposit.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="0" windowWidth="27500" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TrayPlaybackExperimentData" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>FirstHatch(s)</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -1358,8 +1361,8 @@
   <dimension ref="A1:T90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P1" activeCellId="1" sqref="L1:L1048576 P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1494,7 +1497,7 @@
         <v>0.15384615384615385</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="Q2" s="6">
         <v>10.792999999999999</v>
@@ -1557,7 +1560,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="Q3" s="6">
         <v>10.513999999999999</v>
@@ -1607,7 +1610,7 @@
         <v>13</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="M4" s="3">
         <v>0</v>
@@ -1620,7 +1623,7 @@
         <v>0</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="Q4" s="6">
         <v>10.489000000000001</v>
@@ -1670,7 +1673,7 @@
         <v>12</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="M5" s="3">
         <v>0</v>
@@ -1859,7 +1862,7 @@
         <v>14</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="M8" s="3">
         <v>0</v>
@@ -2048,7 +2051,7 @@
         <v>14</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="M11" s="3">
         <v>0</v>
@@ -2237,7 +2240,7 @@
         <v>14</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="M14" s="3">
         <v>0</v>
@@ -2615,7 +2618,7 @@
         <v>15</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="M20" s="3">
         <v>0</v>
@@ -3182,7 +3185,7 @@
         <v>15</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="M29" s="3">
         <v>0</v>
@@ -3195,7 +3198,7 @@
         <v>0</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="Q29" s="9">
         <v>10.476000000000001</v>
@@ -3245,7 +3248,7 @@
         <v>15</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="M30" s="3">
         <v>0</v>
@@ -3308,7 +3311,7 @@
         <v>15</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="M31" s="3">
         <v>0</v>
@@ -3371,7 +3374,7 @@
         <v>15</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="M32" s="3">
         <v>0</v>
@@ -3434,7 +3437,7 @@
         <v>15</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="M33" s="3">
         <v>0</v>
@@ -3497,7 +3500,7 @@
         <v>15</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="M34" s="3">
         <v>0</v>
@@ -4694,7 +4697,7 @@
         <v>11</v>
       </c>
       <c r="L53" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="M53" s="3">
         <v>0</v>
@@ -4757,7 +4760,7 @@
         <v>13</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="M54" s="3">
         <v>0</v>
@@ -4883,7 +4886,7 @@
         <v>14</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="M56" s="3">
         <v>0</v>
@@ -5135,7 +5138,7 @@
         <v>9</v>
       </c>
       <c r="L60" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="M60" s="3">
         <v>0</v>
@@ -5324,7 +5327,7 @@
         <v>12</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="M63" s="3">
         <v>0</v>
@@ -5522,7 +5525,7 @@
         <v>1</v>
       </c>
       <c r="O66" s="8">
-        <f t="shared" ref="O66:O97" si="2">N66/K66</f>
+        <f t="shared" ref="O66:O82" si="2">N66/K66</f>
         <v>0.1111111111111111</v>
       </c>
       <c r="P66" s="3">
@@ -5715,7 +5718,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="P69" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="Q69" s="9">
         <v>11.475</v>
@@ -5778,7 +5781,7 @@
         <v>0.25</v>
       </c>
       <c r="P70" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="Q70" s="9">
         <v>11.816000000000001</v>
@@ -5841,7 +5844,7 @@
         <v>1</v>
       </c>
       <c r="P71" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="Q71" s="9">
         <v>11.612</v>
@@ -6345,7 +6348,7 @@
         <v>0.63636363636363635</v>
       </c>
       <c r="P79" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="Q79" s="9">
         <v>11.813000000000001</v>

</xml_diff>

<commit_message>
up to latency analysis in BoxPlayback.R
added latency in cycles to data
</commit_message>
<xml_diff>
--- a/WarkentinJungRuedaMcDaniel-DataForDeposit.xlsx
+++ b/WarkentinJungRuedaMcDaniel-DataForDeposit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16020" tabRatio="500"/>
+    <workbookView xWindow="2700" yWindow="0" windowWidth="26640" windowHeight="16020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TrayPlaybackExperimentData" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="64">
   <si>
     <t>Date</t>
   </si>
@@ -206,6 +206,12 @@
   <si>
     <t>NA</t>
   </si>
+  <si>
+    <t>CycleLength(s)</t>
+  </si>
+  <si>
+    <t>FirstHatch(cycles)</t>
+  </si>
 </sst>
 </file>
 
@@ -281,8 +287,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="357">
+  <cellStyleXfs count="365">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -672,7 +686,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="357">
+  <cellStyles count="365">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -851,6 +865,10 @@
     <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1029,6 +1047,10 @@
     <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1358,11 +1380,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T90"/>
+  <dimension ref="A1:V82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P1" activeCellId="1" sqref="L1:L1048576 P1:P1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N66" sqref="N66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1378,16 +1400,16 @@
     <col min="9" max="9" width="14" style="11" customWidth="1"/>
     <col min="10" max="10" width="12.83203125" style="11" customWidth="1"/>
     <col min="11" max="11" width="8.6640625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="12" style="3" customWidth="1"/>
-    <col min="13" max="13" width="10.5" style="3" customWidth="1"/>
-    <col min="14" max="14" width="11" style="3" customWidth="1"/>
-    <col min="15" max="15" width="17.33203125" style="8" customWidth="1"/>
-    <col min="16" max="16" width="12" style="3" customWidth="1"/>
-    <col min="17" max="19" width="8.1640625" style="3" customWidth="1"/>
-    <col min="20" max="20" width="11.1640625" style="3" customWidth="1"/>
+    <col min="12" max="14" width="12" style="3" customWidth="1"/>
+    <col min="15" max="15" width="10.5" style="3" customWidth="1"/>
+    <col min="16" max="16" width="11" style="3" customWidth="1"/>
+    <col min="17" max="17" width="17.33203125" style="8" customWidth="1"/>
+    <col min="18" max="18" width="12" style="3" customWidth="1"/>
+    <col min="19" max="21" width="8.1640625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="11.1640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="10" customFormat="1">
+    <row r="1" spans="1:22" s="10" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1425,31 +1447,37 @@
         <v>60</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="1" customFormat="1">
+    <row r="2" spans="1:22" s="1" customFormat="1">
       <c r="A2" s="3">
         <v>20151013</v>
       </c>
@@ -1487,32 +1515,39 @@
         <v>90</v>
       </c>
       <c r="M2" s="3">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="N2" s="3">
-        <v>2</v>
-      </c>
-      <c r="O2" s="8">
-        <f t="shared" ref="O2:O33" si="0">N2/K2</f>
+        <f>L2/M2</f>
+        <v>5.2941176470588234</v>
+      </c>
+      <c r="O2" s="3">
+        <v>2</v>
+      </c>
+      <c r="P2" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="8">
+        <f t="shared" ref="Q2:Q33" si="0">P2/K2</f>
         <v>0.15384615384615385</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="Q2" s="6">
+      <c r="S2" s="6">
         <v>10.792999999999999</v>
       </c>
-      <c r="R2" s="6">
+      <c r="T2" s="6">
         <v>8.1240000000000006</v>
       </c>
-      <c r="S2" s="6">
+      <c r="U2" s="6">
         <v>11.124000000000001</v>
       </c>
-      <c r="T2" s="7">
+      <c r="V2" s="7">
         <v>10.013666666666667</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="1" customFormat="1">
+    <row r="3" spans="1:22" s="1" customFormat="1">
       <c r="A3" s="3">
         <v>20151013</v>
       </c>
@@ -1553,29 +1588,36 @@
         <v>2</v>
       </c>
       <c r="N3" s="3">
-        <v>2</v>
-      </c>
-      <c r="O3" s="8">
+        <f t="shared" ref="N3:N66" si="1">L3/M3</f>
+        <v>39.5</v>
+      </c>
+      <c r="O3" s="3">
+        <v>2</v>
+      </c>
+      <c r="P3" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="8">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="Q3" s="6">
+      <c r="S3" s="6">
         <v>10.513999999999999</v>
       </c>
-      <c r="R3" s="6">
+      <c r="T3" s="6">
         <v>10.698</v>
       </c>
-      <c r="S3" s="6">
+      <c r="U3" s="6">
         <v>11.134</v>
       </c>
-      <c r="T3" s="7">
+      <c r="V3" s="7">
         <v>10.782000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="1" customFormat="1">
+    <row r="4" spans="1:22" s="1" customFormat="1">
       <c r="A4" s="3">
         <v>20151013</v>
       </c>
@@ -1613,32 +1655,38 @@
         <v>61</v>
       </c>
       <c r="M4" s="3">
-        <v>0</v>
-      </c>
-      <c r="N4" s="3">
-        <v>0</v>
-      </c>
-      <c r="O4" s="8">
+        <v>2</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="Q4" s="6">
+      <c r="S4" s="6">
         <v>10.489000000000001</v>
       </c>
-      <c r="R4" s="6">
+      <c r="T4" s="6">
         <v>10.526999999999999</v>
       </c>
-      <c r="S4" s="6">
+      <c r="U4" s="6">
         <v>11</v>
       </c>
-      <c r="T4" s="7">
+      <c r="V4" s="7">
         <v>10.671999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="1" customFormat="1">
+    <row r="5" spans="1:22" s="1" customFormat="1">
       <c r="A5" s="3">
         <v>20151013</v>
       </c>
@@ -1676,32 +1724,38 @@
         <v>61</v>
       </c>
       <c r="M5" s="3">
-        <v>0</v>
-      </c>
-      <c r="N5" s="3">
-        <v>0</v>
-      </c>
-      <c r="O5" s="8">
+        <v>2</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P5" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="6">
+      <c r="R5" s="3">
+        <v>0</v>
+      </c>
+      <c r="S5" s="6">
         <v>10.244</v>
       </c>
-      <c r="R5" s="6">
+      <c r="T5" s="6">
         <v>10.768000000000001</v>
       </c>
-      <c r="S5" s="6">
+      <c r="U5" s="6">
         <v>10.644</v>
       </c>
-      <c r="T5" s="7">
+      <c r="V5" s="7">
         <v>10.552</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="1" customFormat="1">
+    <row r="6" spans="1:22" s="1" customFormat="1">
       <c r="A6" s="3">
         <v>20151013</v>
       </c>
@@ -1739,32 +1793,39 @@
         <v>67</v>
       </c>
       <c r="M6" s="3">
+        <v>17</v>
+      </c>
+      <c r="N6" s="3">
+        <f t="shared" si="1"/>
+        <v>3.9411764705882355</v>
+      </c>
+      <c r="O6" s="3">
         <v>3</v>
       </c>
-      <c r="N6" s="3">
+      <c r="P6" s="3">
         <v>3</v>
       </c>
-      <c r="O6" s="8">
+      <c r="Q6" s="8">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="P6" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="6">
+      <c r="R6" s="3">
+        <v>0</v>
+      </c>
+      <c r="S6" s="6">
         <v>10.654999999999999</v>
       </c>
-      <c r="R6" s="6">
+      <c r="T6" s="6">
         <v>10.346</v>
       </c>
-      <c r="S6" s="6">
+      <c r="U6" s="6">
         <v>11.500999999999999</v>
       </c>
-      <c r="T6" s="7">
+      <c r="V6" s="7">
         <v>10.833999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="1" customFormat="1">
+    <row r="7" spans="1:22" s="1" customFormat="1">
       <c r="A7" s="3">
         <v>20151013</v>
       </c>
@@ -1802,32 +1863,39 @@
         <v>24</v>
       </c>
       <c r="M7" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N7" s="3">
-        <v>2</v>
-      </c>
-      <c r="O7" s="8">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="O7" s="3">
+        <v>1</v>
+      </c>
+      <c r="P7" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="8">
         <f t="shared" si="0"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="P7" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="6">
+      <c r="R7" s="3">
+        <v>1</v>
+      </c>
+      <c r="S7" s="6">
         <v>10.856</v>
       </c>
-      <c r="R7" s="6">
+      <c r="T7" s="6">
         <v>11.157999999999999</v>
       </c>
-      <c r="S7" s="6">
+      <c r="U7" s="6">
         <v>10.323</v>
       </c>
-      <c r="T7" s="7">
+      <c r="V7" s="7">
         <v>10.779000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="1" customFormat="1">
+    <row r="8" spans="1:22" s="1" customFormat="1">
       <c r="A8" s="3">
         <v>20151013</v>
       </c>
@@ -1865,32 +1933,38 @@
         <v>61</v>
       </c>
       <c r="M8" s="3">
-        <v>0</v>
-      </c>
-      <c r="N8" s="3">
-        <v>1</v>
-      </c>
-      <c r="O8" s="8">
+        <v>17</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0</v>
+      </c>
+      <c r="P8" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="8">
         <f t="shared" si="0"/>
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="P8" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="6">
+      <c r="R8" s="3">
+        <v>1</v>
+      </c>
+      <c r="S8" s="6">
         <v>11.510999999999999</v>
       </c>
-      <c r="R8" s="6">
+      <c r="T8" s="6">
         <v>10.928000000000001</v>
       </c>
-      <c r="S8" s="6">
+      <c r="U8" s="6">
         <v>10.782999999999999</v>
       </c>
-      <c r="T8" s="7">
+      <c r="V8" s="7">
         <v>11.074</v>
       </c>
     </row>
-    <row r="9" spans="1:20" s="1" customFormat="1">
+    <row r="9" spans="1:22" s="1" customFormat="1">
       <c r="A9" s="3">
         <v>20151013</v>
       </c>
@@ -1931,29 +2005,36 @@
         <v>2</v>
       </c>
       <c r="N9" s="3">
-        <v>2</v>
-      </c>
-      <c r="O9" s="8">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="O9" s="3">
+        <v>2</v>
+      </c>
+      <c r="P9" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="8">
         <f t="shared" si="0"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="P9" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="6">
+      <c r="R9" s="3">
+        <v>0</v>
+      </c>
+      <c r="S9" s="6">
         <v>10.644</v>
       </c>
-      <c r="R9" s="6">
+      <c r="T9" s="6">
         <v>10.824999999999999</v>
       </c>
-      <c r="S9" s="6">
+      <c r="U9" s="6">
         <v>10.935</v>
       </c>
-      <c r="T9" s="7">
+      <c r="V9" s="7">
         <v>10.801333333333334</v>
       </c>
     </row>
-    <row r="10" spans="1:20" s="1" customFormat="1">
+    <row r="10" spans="1:22" s="1" customFormat="1">
       <c r="A10" s="3">
         <v>20151013</v>
       </c>
@@ -1991,32 +2072,39 @@
         <v>34</v>
       </c>
       <c r="M10" s="3">
+        <v>2</v>
+      </c>
+      <c r="N10" s="3">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="O10" s="3">
         <v>5</v>
       </c>
-      <c r="N10" s="3">
+      <c r="P10" s="3">
         <v>5</v>
       </c>
-      <c r="O10" s="8">
+      <c r="Q10" s="8">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="P10" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="6">
+      <c r="R10" s="3">
+        <v>0</v>
+      </c>
+      <c r="S10" s="6">
         <v>10.695</v>
       </c>
-      <c r="R10" s="6">
+      <c r="T10" s="6">
         <v>10.795</v>
       </c>
-      <c r="S10" s="6">
+      <c r="U10" s="6">
         <v>10.368</v>
       </c>
-      <c r="T10" s="7">
+      <c r="V10" s="7">
         <v>10.619333333333335</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="2" customFormat="1">
+    <row r="11" spans="1:22" s="2" customFormat="1">
       <c r="A11" s="3">
         <v>20151013</v>
       </c>
@@ -2054,32 +2142,38 @@
         <v>61</v>
       </c>
       <c r="M11" s="3">
-        <v>0</v>
-      </c>
-      <c r="N11" s="3">
-        <v>0</v>
-      </c>
-      <c r="O11" s="8">
+        <v>2</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O11" s="3">
+        <v>0</v>
+      </c>
+      <c r="P11" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P11" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="6">
+      <c r="R11" s="3">
+        <v>1</v>
+      </c>
+      <c r="S11" s="6">
         <v>10.641999999999999</v>
       </c>
-      <c r="R11" s="6">
+      <c r="T11" s="6">
         <v>11.125</v>
       </c>
-      <c r="S11" s="6">
+      <c r="U11" s="6">
         <v>11.117000000000001</v>
       </c>
-      <c r="T11" s="7">
+      <c r="V11" s="7">
         <v>10.961333333333334</v>
       </c>
     </row>
-    <row r="12" spans="1:20" s="2" customFormat="1">
+    <row r="12" spans="1:22" s="2" customFormat="1">
       <c r="A12" s="3">
         <v>20151013</v>
       </c>
@@ -2117,32 +2211,39 @@
         <v>210</v>
       </c>
       <c r="M12" s="3">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="N12" s="3">
-        <v>1</v>
-      </c>
-      <c r="O12" s="8">
+        <f t="shared" si="1"/>
+        <v>12.352941176470589</v>
+      </c>
+      <c r="O12" s="3">
+        <v>1</v>
+      </c>
+      <c r="P12" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="8">
         <f t="shared" si="0"/>
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="P12" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="6">
+      <c r="R12" s="3">
+        <v>1</v>
+      </c>
+      <c r="S12" s="6">
         <v>10.29</v>
       </c>
-      <c r="R12" s="6">
+      <c r="T12" s="6">
         <v>11.138</v>
       </c>
-      <c r="S12" s="6">
+      <c r="U12" s="6">
         <v>10.864000000000001</v>
       </c>
-      <c r="T12" s="7">
+      <c r="V12" s="7">
         <v>10.764000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:20" s="2" customFormat="1">
+    <row r="13" spans="1:22" s="2" customFormat="1">
       <c r="A13" s="3">
         <v>20151013</v>
       </c>
@@ -2180,32 +2281,39 @@
         <v>59</v>
       </c>
       <c r="M13" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N13" s="3">
-        <v>1</v>
-      </c>
-      <c r="O13" s="8">
+        <f t="shared" si="1"/>
+        <v>29.5</v>
+      </c>
+      <c r="O13" s="3">
+        <v>1</v>
+      </c>
+      <c r="P13" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="8">
         <f t="shared" si="0"/>
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="P13" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="6">
+      <c r="R13" s="3">
+        <v>1</v>
+      </c>
+      <c r="S13" s="6">
         <v>11.38</v>
       </c>
-      <c r="R13" s="6">
+      <c r="T13" s="6">
         <v>11.398999999999999</v>
       </c>
-      <c r="S13" s="6">
+      <c r="U13" s="6">
         <v>11.599</v>
       </c>
-      <c r="T13" s="7">
+      <c r="V13" s="7">
         <v>11.459333333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:20" s="2" customFormat="1">
+    <row r="14" spans="1:22" s="2" customFormat="1">
       <c r="A14" s="3">
         <v>20151017</v>
       </c>
@@ -2243,32 +2351,38 @@
         <v>61</v>
       </c>
       <c r="M14" s="3">
-        <v>0</v>
-      </c>
-      <c r="N14" s="3">
-        <v>0</v>
-      </c>
-      <c r="O14" s="8">
+        <v>17</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O14" s="3">
+        <v>0</v>
+      </c>
+      <c r="P14" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P14" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="8">
+      <c r="R14" s="3">
+        <v>0</v>
+      </c>
+      <c r="S14" s="8">
         <v>10.566000000000001</v>
       </c>
-      <c r="R14" s="8">
+      <c r="T14" s="8">
         <v>10.595000000000001</v>
       </c>
-      <c r="S14" s="8">
+      <c r="U14" s="8">
         <v>11.526999999999999</v>
       </c>
-      <c r="T14" s="7">
+      <c r="V14" s="7">
         <v>10.896000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:20" s="2" customFormat="1">
+    <row r="15" spans="1:22" s="2" customFormat="1">
       <c r="A15" s="3">
         <v>20151017</v>
       </c>
@@ -2306,32 +2420,39 @@
         <v>19</v>
       </c>
       <c r="M15" s="3">
+        <v>2</v>
+      </c>
+      <c r="N15" s="3">
+        <f t="shared" si="1"/>
+        <v>9.5</v>
+      </c>
+      <c r="O15" s="3">
         <v>10</v>
       </c>
-      <c r="N15" s="3">
+      <c r="P15" s="3">
         <v>10</v>
       </c>
-      <c r="O15" s="8">
+      <c r="Q15" s="8">
         <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P15" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="8">
+      <c r="R15" s="3">
+        <v>1</v>
+      </c>
+      <c r="S15" s="8">
         <v>11.172000000000001</v>
       </c>
-      <c r="R15" s="8">
+      <c r="T15" s="8">
         <v>11.29</v>
       </c>
-      <c r="S15" s="8">
+      <c r="U15" s="8">
         <v>11.772</v>
       </c>
-      <c r="T15" s="7">
+      <c r="V15" s="7">
         <v>11.411333333333333</v>
       </c>
     </row>
-    <row r="16" spans="1:20" s="2" customFormat="1">
+    <row r="16" spans="1:22" s="2" customFormat="1">
       <c r="A16" s="3">
         <v>20151017</v>
       </c>
@@ -2369,32 +2490,39 @@
         <v>160</v>
       </c>
       <c r="M16" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N16" s="3">
-        <v>2</v>
-      </c>
-      <c r="O16" s="8">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="O16" s="3">
+        <v>1</v>
+      </c>
+      <c r="P16" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="8">
         <f t="shared" si="0"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="P16" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="8">
+      <c r="R16" s="3">
+        <v>1</v>
+      </c>
+      <c r="S16" s="8">
         <v>11.010999999999999</v>
       </c>
-      <c r="R16" s="8">
+      <c r="T16" s="8">
         <v>11.379</v>
       </c>
-      <c r="S16" s="8">
+      <c r="U16" s="8">
         <v>11.069000000000001</v>
       </c>
-      <c r="T16" s="7">
+      <c r="V16" s="7">
         <v>11.153</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="2" customFormat="1">
+    <row r="17" spans="1:22" s="2" customFormat="1">
       <c r="A17" s="3">
         <v>20151017</v>
       </c>
@@ -2432,32 +2560,39 @@
         <v>123</v>
       </c>
       <c r="M17" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N17" s="3">
-        <v>1</v>
-      </c>
-      <c r="O17" s="8">
+        <f t="shared" si="1"/>
+        <v>61.5</v>
+      </c>
+      <c r="O17" s="3">
+        <v>1</v>
+      </c>
+      <c r="P17" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="8">
         <f t="shared" si="0"/>
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="P17" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q17" s="8">
+      <c r="R17" s="3">
+        <v>2</v>
+      </c>
+      <c r="S17" s="8">
         <v>11.686</v>
       </c>
-      <c r="R17" s="8">
+      <c r="T17" s="8">
         <v>11.496</v>
       </c>
-      <c r="S17" s="8">
+      <c r="U17" s="8">
         <v>11.55</v>
       </c>
-      <c r="T17" s="7">
+      <c r="V17" s="7">
         <v>11.577333333333334</v>
       </c>
     </row>
-    <row r="18" spans="1:20" s="2" customFormat="1">
+    <row r="18" spans="1:22" s="2" customFormat="1">
       <c r="A18" s="3">
         <v>20151017</v>
       </c>
@@ -2495,32 +2630,39 @@
         <v>25</v>
       </c>
       <c r="M18" s="3">
+        <v>2</v>
+      </c>
+      <c r="N18" s="3">
+        <f t="shared" si="1"/>
+        <v>12.5</v>
+      </c>
+      <c r="O18" s="3">
         <v>8</v>
       </c>
-      <c r="N18" s="3">
+      <c r="P18" s="3">
         <v>8</v>
       </c>
-      <c r="O18" s="8">
+      <c r="Q18" s="8">
         <f t="shared" si="0"/>
         <v>0.5714285714285714</v>
       </c>
-      <c r="P18" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q18" s="8">
+      <c r="R18" s="3">
+        <v>2</v>
+      </c>
+      <c r="S18" s="8">
         <v>11.425000000000001</v>
       </c>
-      <c r="R18" s="8">
+      <c r="T18" s="8">
         <v>11.897</v>
       </c>
-      <c r="S18" s="8">
+      <c r="U18" s="8">
         <v>11.648999999999999</v>
       </c>
-      <c r="T18" s="7">
+      <c r="V18" s="7">
         <v>11.657000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:20" s="2" customFormat="1">
+    <row r="19" spans="1:22" s="2" customFormat="1">
       <c r="A19" s="3">
         <v>20151017</v>
       </c>
@@ -2558,32 +2700,39 @@
         <v>27</v>
       </c>
       <c r="M19" s="3">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="N19" s="3">
-        <v>2</v>
-      </c>
-      <c r="O19" s="8">
+        <f t="shared" si="1"/>
+        <v>1.588235294117647</v>
+      </c>
+      <c r="O19" s="3">
+        <v>2</v>
+      </c>
+      <c r="P19" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q19" s="8">
         <f t="shared" si="0"/>
         <v>0.15384615384615385</v>
       </c>
-      <c r="P19" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="8">
+      <c r="R19" s="3">
+        <v>1</v>
+      </c>
+      <c r="S19" s="8">
         <v>10.782</v>
       </c>
-      <c r="R19" s="8">
+      <c r="T19" s="8">
         <v>11.558</v>
       </c>
-      <c r="S19" s="8">
+      <c r="U19" s="8">
         <v>11.944000000000001</v>
       </c>
-      <c r="T19" s="7">
+      <c r="V19" s="7">
         <v>11.427999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:20" s="1" customFormat="1">
+    <row r="20" spans="1:22" s="1" customFormat="1">
       <c r="A20" s="3">
         <v>20151022</v>
       </c>
@@ -2621,32 +2770,38 @@
         <v>61</v>
       </c>
       <c r="M20" s="3">
-        <v>0</v>
-      </c>
-      <c r="N20" s="3">
-        <v>0</v>
-      </c>
-      <c r="O20" s="8">
+        <v>17</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O20" s="3">
+        <v>0</v>
+      </c>
+      <c r="P20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P20" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q20" s="9">
+      <c r="R20" s="3">
+        <v>2</v>
+      </c>
+      <c r="S20" s="9">
         <v>11.512</v>
       </c>
-      <c r="R20" s="9">
+      <c r="T20" s="9">
         <v>11.287000000000001</v>
       </c>
-      <c r="S20" s="9">
+      <c r="U20" s="9">
         <v>10.974</v>
       </c>
-      <c r="T20" s="7">
+      <c r="V20" s="7">
         <v>11.257666666666665</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="1" customFormat="1">
+    <row r="21" spans="1:22" s="1" customFormat="1">
       <c r="A21" s="3">
         <v>20151022</v>
       </c>
@@ -2684,32 +2839,39 @@
         <v>420</v>
       </c>
       <c r="M21" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N21" s="3">
-        <v>1</v>
-      </c>
-      <c r="O21" s="8">
+        <f t="shared" si="1"/>
+        <v>210</v>
+      </c>
+      <c r="O21" s="3">
+        <v>0</v>
+      </c>
+      <c r="P21" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="8">
         <f t="shared" si="0"/>
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="P21" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q21" s="9">
+      <c r="R21" s="3">
+        <v>2</v>
+      </c>
+      <c r="S21" s="9">
         <v>10.744999999999999</v>
       </c>
-      <c r="R21" s="9">
+      <c r="T21" s="9">
         <v>11.308</v>
       </c>
-      <c r="S21" s="9">
+      <c r="U21" s="9">
         <v>11.236000000000001</v>
       </c>
-      <c r="T21" s="7">
+      <c r="V21" s="7">
         <v>11.096333333333334</v>
       </c>
     </row>
-    <row r="22" spans="1:20" s="1" customFormat="1">
+    <row r="22" spans="1:22" s="1" customFormat="1">
       <c r="A22" s="3">
         <v>20151022</v>
       </c>
@@ -2747,32 +2909,39 @@
         <v>120</v>
       </c>
       <c r="M22" s="3">
+        <v>2</v>
+      </c>
+      <c r="N22" s="3">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="O22" s="3">
         <v>4</v>
       </c>
-      <c r="N22" s="3">
+      <c r="P22" s="3">
         <v>5</v>
       </c>
-      <c r="O22" s="8">
+      <c r="Q22" s="8">
         <f t="shared" si="0"/>
         <v>0.41666666666666669</v>
       </c>
-      <c r="P22" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q22" s="9">
+      <c r="R22" s="3">
+        <v>2</v>
+      </c>
+      <c r="S22" s="9">
         <v>11.365</v>
       </c>
-      <c r="R22" s="9">
+      <c r="T22" s="9">
         <v>11.634</v>
       </c>
-      <c r="S22" s="9">
+      <c r="U22" s="9">
         <v>11.725</v>
       </c>
-      <c r="T22" s="7">
+      <c r="V22" s="7">
         <v>11.574666666666667</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="2" customFormat="1">
+    <row r="23" spans="1:22" s="2" customFormat="1">
       <c r="A23" s="3">
         <v>20151022</v>
       </c>
@@ -2810,32 +2979,39 @@
         <v>251</v>
       </c>
       <c r="M23" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N23" s="3">
-        <v>1</v>
-      </c>
-      <c r="O23" s="8">
+        <f t="shared" si="1"/>
+        <v>125.5</v>
+      </c>
+      <c r="O23" s="3">
+        <v>1</v>
+      </c>
+      <c r="P23" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="8">
         <f t="shared" si="0"/>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="P23" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="9">
+      <c r="R23" s="3">
+        <v>1</v>
+      </c>
+      <c r="S23" s="9">
         <v>11.092000000000001</v>
       </c>
-      <c r="R23" s="9">
+      <c r="T23" s="9">
         <v>11.462999999999999</v>
       </c>
-      <c r="S23" s="9">
+      <c r="U23" s="9">
         <v>11.441000000000001</v>
       </c>
-      <c r="T23" s="7">
+      <c r="V23" s="7">
         <v>11.332000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:20" s="2" customFormat="1">
+    <row r="24" spans="1:22" s="2" customFormat="1">
       <c r="A24" s="3">
         <v>20151022</v>
       </c>
@@ -2873,32 +3049,39 @@
         <v>24</v>
       </c>
       <c r="M24" s="3">
+        <v>2</v>
+      </c>
+      <c r="N24" s="3">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="O24" s="3">
         <v>5</v>
       </c>
-      <c r="N24" s="3">
+      <c r="P24" s="3">
         <v>4</v>
       </c>
-      <c r="O24" s="8">
+      <c r="Q24" s="8">
         <f t="shared" si="0"/>
         <v>0.30769230769230771</v>
       </c>
-      <c r="P24" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q24" s="9">
+      <c r="R24" s="3">
+        <v>2</v>
+      </c>
+      <c r="S24" s="9">
         <v>11.189</v>
       </c>
-      <c r="R24" s="9">
+      <c r="T24" s="9">
         <v>11.462999999999999</v>
       </c>
-      <c r="S24" s="9">
+      <c r="U24" s="9">
         <v>11.961</v>
       </c>
-      <c r="T24" s="7">
+      <c r="V24" s="7">
         <v>11.537666666666667</v>
       </c>
     </row>
-    <row r="25" spans="1:20" s="2" customFormat="1">
+    <row r="25" spans="1:22" s="2" customFormat="1">
       <c r="A25" s="3">
         <v>20151022</v>
       </c>
@@ -2936,32 +3119,39 @@
         <v>64</v>
       </c>
       <c r="M25" s="3">
+        <v>17</v>
+      </c>
+      <c r="N25" s="3">
+        <f t="shared" si="1"/>
+        <v>3.7647058823529411</v>
+      </c>
+      <c r="O25" s="3">
         <v>3</v>
       </c>
-      <c r="N25" s="3">
+      <c r="P25" s="3">
         <v>3</v>
       </c>
-      <c r="O25" s="8">
+      <c r="Q25" s="8">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="P25" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q25" s="9">
+      <c r="R25" s="3">
+        <v>2</v>
+      </c>
+      <c r="S25" s="9">
         <v>11.744</v>
       </c>
-      <c r="R25" s="9">
+      <c r="T25" s="9">
         <v>11.388</v>
       </c>
-      <c r="S25" s="9">
+      <c r="U25" s="9">
         <v>10.945</v>
       </c>
-      <c r="T25" s="7">
+      <c r="V25" s="7">
         <v>11.359</v>
       </c>
     </row>
-    <row r="26" spans="1:20" s="2" customFormat="1">
+    <row r="26" spans="1:22" s="2" customFormat="1">
       <c r="A26" s="3">
         <v>20151022</v>
       </c>
@@ -2999,32 +3189,39 @@
         <v>26</v>
       </c>
       <c r="M26" s="3">
+        <v>2</v>
+      </c>
+      <c r="N26" s="3">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="O26" s="3">
         <v>7</v>
       </c>
-      <c r="N26" s="3">
+      <c r="P26" s="3">
         <v>7</v>
       </c>
-      <c r="O26" s="8">
+      <c r="Q26" s="8">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="P26" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="9">
+      <c r="R26" s="3">
+        <v>1</v>
+      </c>
+      <c r="S26" s="9">
         <v>10.896000000000001</v>
       </c>
-      <c r="R26" s="9">
+      <c r="T26" s="9">
         <v>10.996</v>
       </c>
-      <c r="S26" s="9">
+      <c r="U26" s="9">
         <v>11.234999999999999</v>
       </c>
-      <c r="T26" s="7">
+      <c r="V26" s="7">
         <v>11.042333333333334</v>
       </c>
     </row>
-    <row r="27" spans="1:20" s="2" customFormat="1">
+    <row r="27" spans="1:22" s="2" customFormat="1">
       <c r="A27" s="3">
         <v>20151022</v>
       </c>
@@ -3062,32 +3259,39 @@
         <v>237</v>
       </c>
       <c r="M27" s="3">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="N27" s="3">
-        <v>1</v>
-      </c>
-      <c r="O27" s="8">
+        <f t="shared" si="1"/>
+        <v>13.941176470588236</v>
+      </c>
+      <c r="O27" s="3">
+        <v>1</v>
+      </c>
+      <c r="P27" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="8">
         <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="P27" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q27" s="9">
+      <c r="R27" s="3">
+        <v>1</v>
+      </c>
+      <c r="S27" s="9">
         <v>10.981</v>
       </c>
-      <c r="R27" s="9">
+      <c r="T27" s="9">
         <v>11.718</v>
       </c>
-      <c r="S27" s="9">
+      <c r="U27" s="9">
         <v>11.3</v>
       </c>
-      <c r="T27" s="7">
+      <c r="V27" s="7">
         <v>11.332999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:20" s="2" customFormat="1">
+    <row r="28" spans="1:22" s="2" customFormat="1">
       <c r="A28" s="3">
         <v>20151022</v>
       </c>
@@ -3125,32 +3329,39 @@
         <v>45</v>
       </c>
       <c r="M28" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N28" s="3">
-        <v>2</v>
-      </c>
-      <c r="O28" s="8">
+        <f t="shared" si="1"/>
+        <v>22.5</v>
+      </c>
+      <c r="O28" s="3">
+        <v>1</v>
+      </c>
+      <c r="P28" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q28" s="8">
         <f t="shared" si="0"/>
         <v>0.13333333333333333</v>
       </c>
-      <c r="P28" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q28" s="9">
+      <c r="R28" s="3">
+        <v>2</v>
+      </c>
+      <c r="S28" s="9">
         <v>12.423</v>
       </c>
-      <c r="R28" s="9">
+      <c r="T28" s="9">
         <v>11.836</v>
       </c>
-      <c r="S28" s="9">
+      <c r="U28" s="9">
         <v>11.728999999999999</v>
       </c>
-      <c r="T28" s="7">
+      <c r="V28" s="7">
         <v>11.996</v>
       </c>
     </row>
-    <row r="29" spans="1:20" s="2" customFormat="1">
+    <row r="29" spans="1:22" s="2" customFormat="1">
       <c r="A29" s="3">
         <v>20151025</v>
       </c>
@@ -3188,32 +3399,38 @@
         <v>61</v>
       </c>
       <c r="M29" s="3">
-        <v>0</v>
-      </c>
-      <c r="N29" s="3">
-        <v>0</v>
-      </c>
-      <c r="O29" s="8">
+        <v>17</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O29" s="3">
+        <v>0</v>
+      </c>
+      <c r="P29" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P29" s="3" t="s">
+      <c r="R29" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="Q29" s="9">
+      <c r="S29" s="9">
         <v>10.476000000000001</v>
       </c>
-      <c r="R29" s="9">
+      <c r="T29" s="9">
         <v>10.205</v>
       </c>
-      <c r="S29" s="9">
+      <c r="U29" s="9">
         <v>10.417999999999999</v>
       </c>
-      <c r="T29" s="7">
+      <c r="V29" s="7">
         <v>10.366333333333333</v>
       </c>
     </row>
-    <row r="30" spans="1:20" s="1" customFormat="1">
+    <row r="30" spans="1:22" s="1" customFormat="1">
       <c r="A30" s="3">
         <v>20151025</v>
       </c>
@@ -3251,32 +3468,38 @@
         <v>61</v>
       </c>
       <c r="M30" s="3">
-        <v>0</v>
-      </c>
-      <c r="N30" s="3">
-        <v>0</v>
-      </c>
-      <c r="O30" s="8">
+        <v>2</v>
+      </c>
+      <c r="N30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O30" s="3">
+        <v>0</v>
+      </c>
+      <c r="P30" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P30" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q30" s="9">
+      <c r="R30" s="3">
+        <v>1</v>
+      </c>
+      <c r="S30" s="9">
         <v>10.069000000000001</v>
       </c>
-      <c r="R30" s="9">
+      <c r="T30" s="9">
         <v>10.653</v>
       </c>
-      <c r="S30" s="9">
+      <c r="U30" s="9">
         <v>10.516999999999999</v>
       </c>
-      <c r="T30" s="7">
+      <c r="V30" s="7">
         <v>10.413</v>
       </c>
     </row>
-    <row r="31" spans="1:20" s="1" customFormat="1">
+    <row r="31" spans="1:22" s="1" customFormat="1">
       <c r="A31" s="3">
         <v>20151025</v>
       </c>
@@ -3314,32 +3537,38 @@
         <v>61</v>
       </c>
       <c r="M31" s="3">
-        <v>0</v>
-      </c>
-      <c r="N31" s="3">
-        <v>0</v>
-      </c>
-      <c r="O31" s="8">
+        <v>2</v>
+      </c>
+      <c r="N31" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O31" s="3">
+        <v>0</v>
+      </c>
+      <c r="P31" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P31" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q31" s="9">
+      <c r="R31" s="3">
+        <v>1</v>
+      </c>
+      <c r="S31" s="9">
         <v>10.834</v>
       </c>
-      <c r="R31" s="9">
+      <c r="T31" s="9">
         <v>10.696999999999999</v>
       </c>
-      <c r="S31" s="9">
+      <c r="U31" s="9">
         <v>9.8859999999999992</v>
       </c>
-      <c r="T31" s="7">
+      <c r="V31" s="7">
         <v>10.472333333333333</v>
       </c>
     </row>
-    <row r="32" spans="1:20" s="1" customFormat="1">
+    <row r="32" spans="1:22" s="1" customFormat="1">
       <c r="A32" s="3">
         <v>20151025</v>
       </c>
@@ -3377,32 +3606,38 @@
         <v>61</v>
       </c>
       <c r="M32" s="3">
-        <v>0</v>
-      </c>
-      <c r="N32" s="3">
-        <v>0</v>
-      </c>
-      <c r="O32" s="8">
+        <v>17</v>
+      </c>
+      <c r="N32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O32" s="3">
+        <v>0</v>
+      </c>
+      <c r="P32" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P32" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q32" s="9">
+      <c r="R32" s="3">
+        <v>2</v>
+      </c>
+      <c r="S32" s="9">
         <v>10.336</v>
       </c>
-      <c r="R32" s="9">
+      <c r="T32" s="9">
         <v>10.294</v>
       </c>
-      <c r="S32" s="9">
+      <c r="U32" s="9">
         <v>10.558999999999999</v>
       </c>
-      <c r="T32" s="7">
+      <c r="V32" s="7">
         <v>10.396333333333333</v>
       </c>
     </row>
-    <row r="33" spans="1:20" s="1" customFormat="1">
+    <row r="33" spans="1:22" s="1" customFormat="1">
       <c r="A33" s="3">
         <v>20151025</v>
       </c>
@@ -3440,32 +3675,38 @@
         <v>61</v>
       </c>
       <c r="M33" s="3">
-        <v>0</v>
-      </c>
-      <c r="N33" s="3">
-        <v>0</v>
-      </c>
-      <c r="O33" s="8">
+        <v>2</v>
+      </c>
+      <c r="N33" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O33" s="3">
+        <v>0</v>
+      </c>
+      <c r="P33" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P33" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q33" s="9">
+      <c r="R33" s="3">
+        <v>2</v>
+      </c>
+      <c r="S33" s="9">
         <v>10.701000000000001</v>
       </c>
-      <c r="R33" s="9">
+      <c r="T33" s="9">
         <v>10.753</v>
       </c>
-      <c r="S33" s="9">
+      <c r="U33" s="9">
         <v>10.694000000000001</v>
       </c>
-      <c r="T33" s="7">
+      <c r="V33" s="7">
         <v>10.716000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:20" s="1" customFormat="1">
+    <row r="34" spans="1:22" s="1" customFormat="1">
       <c r="A34" s="3">
         <v>20151025</v>
       </c>
@@ -3503,32 +3744,38 @@
         <v>61</v>
       </c>
       <c r="M34" s="3">
-        <v>0</v>
-      </c>
-      <c r="N34" s="3">
-        <v>0</v>
-      </c>
-      <c r="O34" s="8">
-        <f t="shared" ref="O34:O65" si="1">N34/K34</f>
+        <v>2</v>
+      </c>
+      <c r="N34" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O34" s="3">
         <v>0</v>
       </c>
       <c r="P34" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q34" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="8">
+        <f t="shared" ref="Q34:Q65" si="2">P34/K34</f>
+        <v>0</v>
+      </c>
+      <c r="R34" s="3">
+        <v>1</v>
+      </c>
+      <c r="S34" s="9">
         <v>11.118</v>
       </c>
-      <c r="R34" s="9">
+      <c r="T34" s="9">
         <v>11.164999999999999</v>
       </c>
-      <c r="S34" s="9">
+      <c r="U34" s="9">
         <v>11.316000000000001</v>
       </c>
-      <c r="T34" s="7">
+      <c r="V34" s="7">
         <v>11.199666666666667</v>
       </c>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35" spans="1:22">
       <c r="A35" s="3">
         <v>20151025</v>
       </c>
@@ -3566,32 +3813,39 @@
         <v>124</v>
       </c>
       <c r="M35" s="3">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="N35" s="3">
-        <v>2</v>
-      </c>
-      <c r="O35" s="8">
         <f t="shared" si="1"/>
+        <v>7.2941176470588234</v>
+      </c>
+      <c r="O35" s="3">
+        <v>1</v>
+      </c>
+      <c r="P35" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q35" s="8">
+        <f t="shared" si="2"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="P35" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q35" s="9">
+      <c r="R35" s="3">
+        <v>1</v>
+      </c>
+      <c r="S35" s="9">
         <v>11.169</v>
       </c>
-      <c r="R35" s="9">
+      <c r="T35" s="9">
         <v>11.369</v>
       </c>
-      <c r="S35" s="9">
+      <c r="U35" s="9">
         <v>11.446999999999999</v>
       </c>
-      <c r="T35" s="7">
+      <c r="V35" s="7">
         <v>11.328333333333333</v>
       </c>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:22">
       <c r="A36" s="3">
         <v>20151025</v>
       </c>
@@ -3629,32 +3883,39 @@
         <v>11</v>
       </c>
       <c r="M36" s="3">
+        <v>2</v>
+      </c>
+      <c r="N36" s="3">
+        <f t="shared" si="1"/>
+        <v>5.5</v>
+      </c>
+      <c r="O36" s="3">
         <v>6</v>
       </c>
-      <c r="N36" s="3">
+      <c r="P36" s="3">
         <v>6</v>
       </c>
-      <c r="O36" s="8">
-        <f t="shared" si="1"/>
+      <c r="Q36" s="8">
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="P36" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q36" s="9">
+      <c r="R36" s="3">
+        <v>1</v>
+      </c>
+      <c r="S36" s="9">
         <v>11.052</v>
       </c>
-      <c r="R36" s="9">
+      <c r="T36" s="9">
         <v>11.28</v>
       </c>
-      <c r="S36" s="9">
+      <c r="U36" s="9">
         <v>11.265000000000001</v>
       </c>
-      <c r="T36" s="7">
+      <c r="V36" s="7">
         <v>11.199</v>
       </c>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37" spans="1:22">
       <c r="A37" s="3">
         <v>20151025</v>
       </c>
@@ -3692,32 +3953,39 @@
         <v>231</v>
       </c>
       <c r="M37" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N37" s="3">
-        <v>1</v>
-      </c>
-      <c r="O37" s="8">
         <f t="shared" si="1"/>
+        <v>115.5</v>
+      </c>
+      <c r="O37" s="3">
+        <v>1</v>
+      </c>
+      <c r="P37" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="8">
+        <f t="shared" si="2"/>
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="P37" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q37" s="9">
+      <c r="R37" s="3">
+        <v>1</v>
+      </c>
+      <c r="S37" s="9">
         <v>11.935</v>
       </c>
-      <c r="R37" s="9">
+      <c r="T37" s="9">
         <v>12.103999999999999</v>
       </c>
-      <c r="S37" s="9">
+      <c r="U37" s="9">
         <v>11.664</v>
       </c>
-      <c r="T37" s="7">
+      <c r="V37" s="7">
         <v>11.901000000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:20">
+    <row r="38" spans="1:22">
       <c r="A38" s="3">
         <v>20151026</v>
       </c>
@@ -3755,32 +4023,39 @@
         <v>13</v>
       </c>
       <c r="M38" s="3">
+        <v>2</v>
+      </c>
+      <c r="N38" s="3">
+        <f t="shared" si="1"/>
+        <v>6.5</v>
+      </c>
+      <c r="O38" s="3">
         <v>8</v>
       </c>
-      <c r="N38" s="3">
+      <c r="P38" s="3">
         <v>8</v>
       </c>
-      <c r="O38" s="8">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="P38" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q38" s="9">
+      <c r="Q38" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="R38" s="3">
+        <v>2</v>
+      </c>
+      <c r="S38" s="9">
         <v>11.17</v>
       </c>
-      <c r="R38" s="9">
+      <c r="T38" s="9">
         <v>10.932</v>
       </c>
-      <c r="S38" s="3" t="s">
+      <c r="U38" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="T38" s="7">
+      <c r="V38" s="7">
         <v>11.051</v>
       </c>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39" spans="1:22">
       <c r="A39" s="3">
         <v>20151026</v>
       </c>
@@ -3818,32 +4093,39 @@
         <v>45</v>
       </c>
       <c r="M39" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N39" s="3">
-        <v>1</v>
-      </c>
-      <c r="O39" s="8">
         <f t="shared" si="1"/>
+        <v>22.5</v>
+      </c>
+      <c r="O39" s="3">
+        <v>1</v>
+      </c>
+      <c r="P39" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="8">
+        <f t="shared" si="2"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="P39" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q39" s="9">
+      <c r="R39" s="3">
+        <v>2</v>
+      </c>
+      <c r="S39" s="9">
         <v>11.759</v>
       </c>
-      <c r="R39" s="9">
+      <c r="T39" s="9">
         <v>11.446999999999999</v>
       </c>
-      <c r="S39" s="9">
+      <c r="U39" s="9">
         <v>10.375999999999999</v>
       </c>
-      <c r="T39" s="7">
+      <c r="V39" s="7">
         <v>11.194000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:22">
       <c r="A40" s="3">
         <v>20151026</v>
       </c>
@@ -3881,32 +4163,39 @@
         <v>69</v>
       </c>
       <c r="M40" s="3">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="N40" s="3">
-        <v>2</v>
-      </c>
-      <c r="O40" s="8">
         <f t="shared" si="1"/>
+        <v>4.0588235294117645</v>
+      </c>
+      <c r="O40" s="3">
+        <v>2</v>
+      </c>
+      <c r="P40" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q40" s="8">
+        <f t="shared" si="2"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="P40" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q40" s="9">
+      <c r="R40" s="3">
+        <v>2</v>
+      </c>
+      <c r="S40" s="9">
         <v>11.318</v>
       </c>
-      <c r="R40" s="9">
+      <c r="T40" s="9">
         <v>10.778</v>
       </c>
-      <c r="S40" s="9">
+      <c r="U40" s="9">
         <v>11.958</v>
       </c>
-      <c r="T40" s="7">
+      <c r="V40" s="7">
         <v>11.351333333333335</v>
       </c>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:22">
       <c r="A41" s="3">
         <v>20151013</v>
       </c>
@@ -3944,32 +4233,39 @@
         <v>34</v>
       </c>
       <c r="M41" s="3">
+        <v>2</v>
+      </c>
+      <c r="N41" s="3">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="O41" s="3">
         <v>3</v>
       </c>
-      <c r="N41" s="3">
+      <c r="P41" s="3">
         <v>4</v>
       </c>
-      <c r="O41" s="8">
-        <f t="shared" si="1"/>
+      <c r="Q41" s="8">
+        <f t="shared" si="2"/>
         <v>0.44444444444444442</v>
       </c>
-      <c r="P41" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q41" s="6">
+      <c r="R41" s="3">
+        <v>2</v>
+      </c>
+      <c r="S41" s="6">
         <v>11.541</v>
       </c>
-      <c r="R41" s="6">
+      <c r="T41" s="6">
         <v>11.752000000000001</v>
       </c>
-      <c r="S41" s="6">
+      <c r="U41" s="6">
         <v>11.742000000000001</v>
       </c>
-      <c r="T41" s="7">
+      <c r="V41" s="7">
         <v>11.678333333333333</v>
       </c>
     </row>
-    <row r="42" spans="1:20">
+    <row r="42" spans="1:22">
       <c r="A42" s="3">
         <v>20151013</v>
       </c>
@@ -4007,32 +4303,39 @@
         <v>14</v>
       </c>
       <c r="M42" s="3">
+        <v>17</v>
+      </c>
+      <c r="N42" s="3">
+        <f t="shared" si="1"/>
+        <v>0.82352941176470584</v>
+      </c>
+      <c r="O42" s="3">
         <v>10</v>
       </c>
-      <c r="N42" s="3">
+      <c r="P42" s="3">
         <v>10</v>
       </c>
-      <c r="O42" s="8">
-        <f t="shared" si="1"/>
+      <c r="Q42" s="8">
+        <f t="shared" si="2"/>
         <v>0.7142857142857143</v>
       </c>
-      <c r="P42" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q42" s="6">
+      <c r="R42" s="3">
+        <v>1</v>
+      </c>
+      <c r="S42" s="6">
         <v>11.374000000000001</v>
       </c>
-      <c r="R42" s="6">
+      <c r="T42" s="6">
         <v>10.959</v>
       </c>
-      <c r="S42" s="6">
+      <c r="U42" s="6">
         <v>11.068</v>
       </c>
-      <c r="T42" s="7">
+      <c r="V42" s="7">
         <v>11.133666666666665</v>
       </c>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43" spans="1:22">
       <c r="A43" s="3">
         <v>20151013</v>
       </c>
@@ -4070,32 +4373,39 @@
         <v>25</v>
       </c>
       <c r="M43" s="3">
+        <v>2</v>
+      </c>
+      <c r="N43" s="3">
+        <f t="shared" si="1"/>
+        <v>12.5</v>
+      </c>
+      <c r="O43" s="3">
         <v>3</v>
       </c>
-      <c r="N43" s="3">
+      <c r="P43" s="3">
         <v>3</v>
       </c>
-      <c r="O43" s="8">
-        <f t="shared" si="1"/>
+      <c r="Q43" s="8">
+        <f t="shared" si="2"/>
         <v>0.21428571428571427</v>
       </c>
-      <c r="P43" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q43" s="6">
+      <c r="R43" s="3">
+        <v>1</v>
+      </c>
+      <c r="S43" s="6">
         <v>10.965</v>
       </c>
-      <c r="R43" s="6">
+      <c r="T43" s="6">
         <v>11.529</v>
       </c>
-      <c r="S43" s="6">
+      <c r="U43" s="6">
         <v>11.247</v>
       </c>
-      <c r="T43" s="7">
+      <c r="V43" s="7">
         <v>11.247</v>
       </c>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44" spans="1:22">
       <c r="A44" s="3">
         <v>20151013</v>
       </c>
@@ -4133,32 +4443,39 @@
         <v>95</v>
       </c>
       <c r="M44" s="3">
+        <v>2</v>
+      </c>
+      <c r="N44" s="3">
+        <f t="shared" si="1"/>
+        <v>47.5</v>
+      </c>
+      <c r="O44" s="3">
         <v>4</v>
       </c>
-      <c r="N44" s="3">
+      <c r="P44" s="3">
         <v>4</v>
       </c>
-      <c r="O44" s="8">
-        <f t="shared" si="1"/>
+      <c r="Q44" s="8">
+        <f t="shared" si="2"/>
         <v>0.4</v>
       </c>
-      <c r="P44" s="3">
+      <c r="R44" s="3">
         <v>3</v>
       </c>
-      <c r="Q44" s="6">
+      <c r="S44" s="6">
         <v>11.805</v>
       </c>
-      <c r="R44" s="6">
+      <c r="T44" s="6">
         <v>11.942</v>
       </c>
-      <c r="S44" s="6">
+      <c r="U44" s="6">
         <v>11.409000000000001</v>
       </c>
-      <c r="T44" s="7">
+      <c r="V44" s="7">
         <v>11.718666666666666</v>
       </c>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:22">
       <c r="A45" s="3">
         <v>20151013</v>
       </c>
@@ -4196,32 +4513,39 @@
         <v>12</v>
       </c>
       <c r="M45" s="3">
+        <v>2</v>
+      </c>
+      <c r="N45" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="O45" s="3">
         <v>10</v>
       </c>
-      <c r="N45" s="3">
+      <c r="P45" s="3">
         <v>10</v>
       </c>
-      <c r="O45" s="8">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="P45" s="3">
+      <c r="Q45" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="R45" s="3">
         <v>3</v>
       </c>
-      <c r="Q45" s="6">
+      <c r="S45" s="6">
         <v>11.811999999999999</v>
       </c>
-      <c r="R45" s="6">
+      <c r="T45" s="6">
         <v>11.654</v>
       </c>
-      <c r="S45" s="6">
+      <c r="U45" s="6">
         <v>11.38</v>
       </c>
-      <c r="T45" s="7">
+      <c r="V45" s="7">
         <v>11.615333333333334</v>
       </c>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46" spans="1:22">
       <c r="A46" s="3">
         <v>20151013</v>
       </c>
@@ -4259,32 +4583,39 @@
         <v>32</v>
       </c>
       <c r="M46" s="3">
+        <v>17</v>
+      </c>
+      <c r="N46" s="3">
+        <f t="shared" si="1"/>
+        <v>1.8823529411764706</v>
+      </c>
+      <c r="O46" s="3">
         <v>12</v>
       </c>
-      <c r="N46" s="3">
+      <c r="P46" s="3">
         <v>12</v>
       </c>
-      <c r="O46" s="8">
-        <f t="shared" si="1"/>
+      <c r="Q46" s="8">
+        <f t="shared" si="2"/>
         <v>0.92307692307692313</v>
       </c>
-      <c r="P46" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q46" s="6">
+      <c r="R46" s="3">
+        <v>2</v>
+      </c>
+      <c r="S46" s="6">
         <v>11.65</v>
       </c>
-      <c r="R46" s="6">
+      <c r="T46" s="6">
         <v>11.994</v>
       </c>
-      <c r="S46" s="6">
+      <c r="U46" s="6">
         <v>11.4</v>
       </c>
-      <c r="T46" s="7">
+      <c r="V46" s="7">
         <v>11.681333333333333</v>
       </c>
     </row>
-    <row r="47" spans="1:20" s="1" customFormat="1">
+    <row r="47" spans="1:22" s="1" customFormat="1">
       <c r="A47" s="3">
         <v>20151013</v>
       </c>
@@ -4322,32 +4653,39 @@
         <v>45</v>
       </c>
       <c r="M47" s="3">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="N47" s="3">
-        <v>2</v>
-      </c>
-      <c r="O47" s="8">
         <f t="shared" si="1"/>
+        <v>2.6470588235294117</v>
+      </c>
+      <c r="O47" s="3">
+        <v>2</v>
+      </c>
+      <c r="P47" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q47" s="8">
+        <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
-      <c r="P47" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q47" s="6">
+      <c r="R47" s="3">
+        <v>2</v>
+      </c>
+      <c r="S47" s="6">
         <v>11.984999999999999</v>
       </c>
-      <c r="R47" s="6">
+      <c r="T47" s="6">
         <v>11.949</v>
       </c>
-      <c r="S47" s="6">
+      <c r="U47" s="6">
         <v>11.872</v>
       </c>
-      <c r="T47" s="7">
+      <c r="V47" s="7">
         <v>11.935333333333332</v>
       </c>
     </row>
-    <row r="48" spans="1:20" s="1" customFormat="1">
+    <row r="48" spans="1:22" s="1" customFormat="1">
       <c r="A48" s="3">
         <v>20151013</v>
       </c>
@@ -4388,29 +4726,36 @@
         <v>2</v>
       </c>
       <c r="N48" s="3">
-        <v>3</v>
-      </c>
-      <c r="O48" s="8">
         <f t="shared" si="1"/>
-        <v>0.27272727272727271</v>
+        <v>13.5</v>
+      </c>
+      <c r="O48" s="3">
+        <v>2</v>
       </c>
       <c r="P48" s="3">
         <v>3</v>
       </c>
-      <c r="Q48" s="6">
+      <c r="Q48" s="8">
+        <f t="shared" si="2"/>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="R48" s="3">
+        <v>3</v>
+      </c>
+      <c r="S48" s="6">
         <v>11.263999999999999</v>
       </c>
-      <c r="R48" s="6">
+      <c r="T48" s="6">
         <v>12.146000000000001</v>
       </c>
-      <c r="S48" s="6">
+      <c r="U48" s="6">
         <v>11.621</v>
       </c>
-      <c r="T48" s="7">
+      <c r="V48" s="7">
         <v>11.677</v>
       </c>
     </row>
-    <row r="49" spans="1:20" s="1" customFormat="1">
+    <row r="49" spans="1:22" s="1" customFormat="1">
       <c r="A49" s="3">
         <v>20151013</v>
       </c>
@@ -4448,32 +4793,39 @@
         <v>30</v>
       </c>
       <c r="M49" s="3">
+        <v>2</v>
+      </c>
+      <c r="N49" s="3">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="O49" s="3">
         <v>6</v>
       </c>
-      <c r="N49" s="3">
+      <c r="P49" s="3">
         <v>6</v>
       </c>
-      <c r="O49" s="8">
-        <f t="shared" si="1"/>
+      <c r="Q49" s="8">
+        <f t="shared" si="2"/>
         <v>0.42857142857142855</v>
       </c>
-      <c r="P49" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q49" s="6">
+      <c r="R49" s="3">
+        <v>2</v>
+      </c>
+      <c r="S49" s="6">
         <v>10.62</v>
       </c>
-      <c r="R49" s="6">
+      <c r="T49" s="6">
         <v>11.074</v>
       </c>
-      <c r="S49" s="6">
+      <c r="U49" s="6">
         <v>11.058</v>
       </c>
-      <c r="T49" s="7">
+      <c r="V49" s="7">
         <v>10.917333333333332</v>
       </c>
     </row>
-    <row r="50" spans="1:20" s="1" customFormat="1">
+    <row r="50" spans="1:22" s="1" customFormat="1">
       <c r="A50" s="3">
         <v>20151013</v>
       </c>
@@ -4514,29 +4866,36 @@
         <v>2</v>
       </c>
       <c r="N50" s="3">
-        <v>3</v>
-      </c>
-      <c r="O50" s="8">
         <f t="shared" si="1"/>
-        <v>0.21428571428571427</v>
+        <v>18</v>
+      </c>
+      <c r="O50" s="3">
+        <v>2</v>
       </c>
       <c r="P50" s="3">
         <v>3</v>
       </c>
-      <c r="Q50" s="6">
+      <c r="Q50" s="8">
+        <f t="shared" si="2"/>
+        <v>0.21428571428571427</v>
+      </c>
+      <c r="R50" s="3">
+        <v>3</v>
+      </c>
+      <c r="S50" s="6">
         <v>12.301</v>
       </c>
-      <c r="R50" s="6">
+      <c r="T50" s="6">
         <v>11.935</v>
       </c>
-      <c r="S50" s="6">
+      <c r="U50" s="6">
         <v>11.545999999999999</v>
       </c>
-      <c r="T50" s="7">
+      <c r="V50" s="7">
         <v>11.927333333333332</v>
       </c>
     </row>
-    <row r="51" spans="1:20" s="1" customFormat="1">
+    <row r="51" spans="1:22" s="1" customFormat="1">
       <c r="A51" s="3">
         <v>20151013</v>
       </c>
@@ -4574,32 +4933,39 @@
         <v>15</v>
       </c>
       <c r="M51" s="3">
+        <v>2</v>
+      </c>
+      <c r="N51" s="3">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+      <c r="O51" s="3">
         <v>10</v>
       </c>
-      <c r="N51" s="3">
+      <c r="P51" s="3">
         <v>10</v>
       </c>
-      <c r="O51" s="8">
-        <f t="shared" si="1"/>
+      <c r="Q51" s="8">
+        <f t="shared" si="2"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P51" s="3">
+      <c r="R51" s="3">
         <v>3</v>
       </c>
-      <c r="Q51" s="6">
+      <c r="S51" s="6">
         <v>11.965999999999999</v>
       </c>
-      <c r="R51" s="6">
+      <c r="T51" s="6">
         <v>12.2</v>
       </c>
-      <c r="S51" s="6">
+      <c r="U51" s="6">
         <v>12.14</v>
       </c>
-      <c r="T51" s="7">
+      <c r="V51" s="7">
         <v>12.101999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:20" s="1" customFormat="1">
+    <row r="52" spans="1:22" s="1" customFormat="1">
       <c r="A52" s="3">
         <v>20151013</v>
       </c>
@@ -4637,32 +5003,39 @@
         <v>29</v>
       </c>
       <c r="M52" s="3">
+        <v>17</v>
+      </c>
+      <c r="N52" s="3">
+        <f t="shared" si="1"/>
+        <v>1.7058823529411764</v>
+      </c>
+      <c r="O52" s="3">
         <v>12</v>
       </c>
-      <c r="N52" s="3">
+      <c r="P52" s="3">
         <v>12</v>
       </c>
-      <c r="O52" s="8">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="P52" s="3">
+      <c r="Q52" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="R52" s="3">
         <v>3</v>
       </c>
-      <c r="Q52" s="6">
+      <c r="S52" s="6">
         <v>11.35</v>
       </c>
-      <c r="R52" s="6">
+      <c r="T52" s="6">
         <v>11.885</v>
       </c>
-      <c r="S52" s="6">
+      <c r="U52" s="6">
         <v>11.84</v>
       </c>
-      <c r="T52" s="7">
+      <c r="V52" s="7">
         <v>11.691666666666668</v>
       </c>
     </row>
-    <row r="53" spans="1:20" s="1" customFormat="1">
+    <row r="53" spans="1:22" s="1" customFormat="1">
       <c r="A53" s="3">
         <v>20151013</v>
       </c>
@@ -4700,32 +5073,38 @@
         <v>61</v>
       </c>
       <c r="M53" s="3">
-        <v>0</v>
-      </c>
-      <c r="N53" s="3">
-        <v>0</v>
-      </c>
-      <c r="O53" s="8">
-        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="N53" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O53" s="3">
         <v>0</v>
       </c>
       <c r="P53" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R53" s="3">
         <v>3</v>
       </c>
-      <c r="Q53" s="6">
+      <c r="S53" s="6">
         <v>10.365</v>
       </c>
-      <c r="R53" s="6">
+      <c r="T53" s="6">
         <v>11.467000000000001</v>
       </c>
-      <c r="S53" s="6">
+      <c r="U53" s="6">
         <v>11.52</v>
       </c>
-      <c r="T53" s="7">
+      <c r="V53" s="7">
         <v>11.117333333333335</v>
       </c>
     </row>
-    <row r="54" spans="1:20" s="1" customFormat="1">
+    <row r="54" spans="1:22" s="1" customFormat="1">
       <c r="A54" s="3">
         <v>20151013</v>
       </c>
@@ -4763,32 +5142,38 @@
         <v>61</v>
       </c>
       <c r="M54" s="3">
-        <v>0</v>
-      </c>
-      <c r="N54" s="3">
-        <v>0</v>
-      </c>
-      <c r="O54" s="8">
-        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="N54" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O54" s="3">
         <v>0</v>
       </c>
       <c r="P54" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q54" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R54" s="3">
+        <v>2</v>
+      </c>
+      <c r="S54" s="6">
         <v>10.653</v>
       </c>
-      <c r="R54" s="6">
+      <c r="T54" s="6">
         <v>10.679</v>
       </c>
-      <c r="S54" s="6">
+      <c r="U54" s="6">
         <v>10.795</v>
       </c>
-      <c r="T54" s="7">
+      <c r="V54" s="7">
         <v>10.709000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:20" s="1" customFormat="1">
+    <row r="55" spans="1:22" s="1" customFormat="1">
       <c r="A55" s="3">
         <v>20151013</v>
       </c>
@@ -4826,32 +5211,39 @@
         <v>21</v>
       </c>
       <c r="M55" s="3">
+        <v>2</v>
+      </c>
+      <c r="N55" s="3">
+        <f t="shared" si="1"/>
+        <v>10.5</v>
+      </c>
+      <c r="O55" s="3">
         <v>5</v>
       </c>
-      <c r="N55" s="3">
+      <c r="P55" s="3">
         <v>5</v>
       </c>
-      <c r="O55" s="8">
-        <f t="shared" si="1"/>
+      <c r="Q55" s="8">
+        <f t="shared" si="2"/>
         <v>0.38461538461538464</v>
       </c>
-      <c r="P55" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q55" s="6">
+      <c r="R55" s="3">
+        <v>2</v>
+      </c>
+      <c r="S55" s="6">
         <v>11.701000000000001</v>
       </c>
-      <c r="R55" s="6">
+      <c r="T55" s="6">
         <v>11.16</v>
       </c>
-      <c r="S55" s="6">
+      <c r="U55" s="6">
         <v>11.561</v>
       </c>
-      <c r="T55" s="7">
+      <c r="V55" s="7">
         <v>11.473999999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:20">
+    <row r="56" spans="1:22">
       <c r="A56" s="3">
         <v>20151017</v>
       </c>
@@ -4889,32 +5281,38 @@
         <v>61</v>
       </c>
       <c r="M56" s="3">
-        <v>0</v>
-      </c>
-      <c r="N56" s="3">
-        <v>0</v>
-      </c>
-      <c r="O56" s="8">
-        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="N56" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O56" s="3">
         <v>0</v>
       </c>
       <c r="P56" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R56" s="3">
         <v>3</v>
       </c>
-      <c r="Q56" s="8">
+      <c r="S56" s="8">
         <v>12.276999999999999</v>
       </c>
-      <c r="R56" s="8">
+      <c r="T56" s="8">
         <v>11.797000000000001</v>
       </c>
-      <c r="S56" s="8">
+      <c r="U56" s="8">
         <v>11.491</v>
       </c>
-      <c r="T56" s="7">
+      <c r="V56" s="7">
         <v>11.854999999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:20">
+    <row r="57" spans="1:22">
       <c r="A57" s="3">
         <v>20151017</v>
       </c>
@@ -4952,32 +5350,39 @@
         <v>70</v>
       </c>
       <c r="M57" s="3">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="N57" s="3">
-        <v>1</v>
-      </c>
-      <c r="O57" s="8">
         <f t="shared" si="1"/>
+        <v>4.117647058823529</v>
+      </c>
+      <c r="O57" s="3">
+        <v>1</v>
+      </c>
+      <c r="P57" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q57" s="8">
+        <f t="shared" si="2"/>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="P57" s="3">
+      <c r="R57" s="3">
         <v>3</v>
       </c>
-      <c r="Q57" s="8">
+      <c r="S57" s="8">
         <v>11.696999999999999</v>
       </c>
-      <c r="R57" s="8">
+      <c r="T57" s="8">
         <v>11.814</v>
       </c>
-      <c r="S57" s="8">
+      <c r="U57" s="8">
         <v>11.638</v>
       </c>
-      <c r="T57" s="7">
+      <c r="V57" s="7">
         <v>11.716333333333333</v>
       </c>
     </row>
-    <row r="58" spans="1:20">
+    <row r="58" spans="1:22">
       <c r="A58" s="3">
         <v>20151017</v>
       </c>
@@ -5015,32 +5420,39 @@
         <v>17</v>
       </c>
       <c r="M58" s="3">
+        <v>2</v>
+      </c>
+      <c r="N58" s="3">
+        <f t="shared" si="1"/>
+        <v>8.5</v>
+      </c>
+      <c r="O58" s="3">
         <v>6</v>
       </c>
-      <c r="N58" s="3">
+      <c r="P58" s="3">
         <v>6</v>
       </c>
-      <c r="O58" s="8">
-        <f t="shared" si="1"/>
+      <c r="Q58" s="8">
+        <f t="shared" si="2"/>
         <v>0.42857142857142855</v>
       </c>
-      <c r="P58" s="3">
+      <c r="R58" s="3">
         <v>3</v>
       </c>
-      <c r="Q58" s="8">
+      <c r="S58" s="8">
         <v>11.603</v>
       </c>
-      <c r="R58" s="8">
+      <c r="T58" s="8">
         <v>11.867000000000001</v>
       </c>
-      <c r="S58" s="8">
+      <c r="U58" s="8">
         <v>11.396000000000001</v>
       </c>
-      <c r="T58" s="7">
+      <c r="V58" s="7">
         <v>11.622</v>
       </c>
     </row>
-    <row r="59" spans="1:20">
+    <row r="59" spans="1:22">
       <c r="A59" s="3">
         <v>20151017</v>
       </c>
@@ -5078,32 +5490,39 @@
         <v>34</v>
       </c>
       <c r="M59" s="3">
+        <v>17</v>
+      </c>
+      <c r="N59" s="3">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="O59" s="3">
         <v>4</v>
       </c>
-      <c r="N59" s="3">
+      <c r="P59" s="3">
         <v>4</v>
       </c>
-      <c r="O59" s="8">
-        <f t="shared" si="1"/>
+      <c r="Q59" s="8">
+        <f t="shared" si="2"/>
         <v>0.36363636363636365</v>
       </c>
-      <c r="P59" s="3">
+      <c r="R59" s="3">
         <v>3</v>
       </c>
-      <c r="Q59" s="8">
+      <c r="S59" s="8">
         <v>12.12</v>
       </c>
-      <c r="R59" s="8">
+      <c r="T59" s="8">
         <v>11.521000000000001</v>
       </c>
-      <c r="S59" s="8">
+      <c r="U59" s="8">
         <v>11.911</v>
       </c>
-      <c r="T59" s="7">
+      <c r="V59" s="7">
         <v>11.850666666666667</v>
       </c>
     </row>
-    <row r="60" spans="1:20">
+    <row r="60" spans="1:22">
       <c r="A60" s="3">
         <v>20151017</v>
       </c>
@@ -5141,32 +5560,38 @@
         <v>61</v>
       </c>
       <c r="M60" s="3">
-        <v>0</v>
-      </c>
-      <c r="N60" s="3">
-        <v>0</v>
-      </c>
-      <c r="O60" s="8">
-        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="N60" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O60" s="3">
         <v>0</v>
       </c>
       <c r="P60" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R60" s="3">
         <v>3</v>
       </c>
-      <c r="Q60" s="8">
+      <c r="S60" s="8">
         <v>11.721</v>
       </c>
-      <c r="R60" s="8">
+      <c r="T60" s="8">
         <v>10.538</v>
       </c>
-      <c r="S60" s="8">
+      <c r="U60" s="8">
         <v>11.997999999999999</v>
       </c>
-      <c r="T60" s="7">
+      <c r="V60" s="7">
         <v>11.418999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:20">
+    <row r="61" spans="1:22">
       <c r="A61" s="3">
         <v>20151017</v>
       </c>
@@ -5204,32 +5629,39 @@
         <v>23</v>
       </c>
       <c r="M61" s="3">
+        <v>2</v>
+      </c>
+      <c r="N61" s="3">
+        <f t="shared" si="1"/>
+        <v>11.5</v>
+      </c>
+      <c r="O61" s="3">
         <v>5</v>
       </c>
-      <c r="N61" s="3">
+      <c r="P61" s="3">
         <v>6</v>
       </c>
-      <c r="O61" s="8">
-        <f t="shared" si="1"/>
+      <c r="Q61" s="8">
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
-      <c r="P61" s="3">
+      <c r="R61" s="3">
         <v>3</v>
       </c>
-      <c r="Q61" s="8">
+      <c r="S61" s="8">
         <v>10.615</v>
       </c>
-      <c r="R61" s="8">
+      <c r="T61" s="8">
         <v>11.72</v>
       </c>
-      <c r="S61" s="8">
+      <c r="U61" s="8">
         <v>11.499000000000001</v>
       </c>
-      <c r="T61" s="7">
+      <c r="V61" s="7">
         <v>11.278</v>
       </c>
     </row>
-    <row r="62" spans="1:20" s="1" customFormat="1">
+    <row r="62" spans="1:22" s="1" customFormat="1">
       <c r="A62" s="3">
         <v>20151017</v>
       </c>
@@ -5267,32 +5699,39 @@
         <v>16</v>
       </c>
       <c r="M62" s="3">
+        <v>2</v>
+      </c>
+      <c r="N62" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="O62" s="3">
         <v>6</v>
       </c>
-      <c r="N62" s="3">
+      <c r="P62" s="3">
         <v>6</v>
       </c>
-      <c r="O62" s="8">
-        <f t="shared" si="1"/>
+      <c r="Q62" s="8">
+        <f t="shared" si="2"/>
         <v>0.42857142857142855</v>
       </c>
-      <c r="P62" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q62" s="8">
+      <c r="R62" s="3">
+        <v>2</v>
+      </c>
+      <c r="S62" s="8">
         <v>11.558</v>
       </c>
-      <c r="R62" s="8">
+      <c r="T62" s="8">
         <v>11.714</v>
       </c>
-      <c r="S62" s="8">
+      <c r="U62" s="8">
         <v>11.821999999999999</v>
       </c>
-      <c r="T62" s="7">
+      <c r="V62" s="7">
         <v>11.697999999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:20" s="1" customFormat="1">
+    <row r="63" spans="1:22" s="1" customFormat="1">
       <c r="A63" s="3">
         <v>20151017</v>
       </c>
@@ -5330,32 +5769,38 @@
         <v>61</v>
       </c>
       <c r="M63" s="3">
-        <v>0</v>
-      </c>
-      <c r="N63" s="3">
-        <v>0</v>
-      </c>
-      <c r="O63" s="8">
-        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="N63" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O63" s="3">
         <v>0</v>
       </c>
       <c r="P63" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q63" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R63" s="3">
         <v>3</v>
       </c>
-      <c r="Q63" s="8">
+      <c r="S63" s="8">
         <v>12.128</v>
       </c>
-      <c r="R63" s="8">
+      <c r="T63" s="8">
         <v>12.132999999999999</v>
       </c>
-      <c r="S63" s="8">
+      <c r="U63" s="8">
         <v>11.944000000000001</v>
       </c>
-      <c r="T63" s="7">
+      <c r="V63" s="7">
         <v>12.068333333333333</v>
       </c>
     </row>
-    <row r="64" spans="1:20" s="1" customFormat="1">
+    <row r="64" spans="1:22" s="1" customFormat="1">
       <c r="A64" s="3">
         <v>20151017</v>
       </c>
@@ -5393,32 +5838,39 @@
         <v>25</v>
       </c>
       <c r="M64" s="3">
+        <v>17</v>
+      </c>
+      <c r="N64" s="3">
+        <f t="shared" si="1"/>
+        <v>1.4705882352941178</v>
+      </c>
+      <c r="O64" s="3">
         <v>11</v>
       </c>
-      <c r="N64" s="3">
+      <c r="P64" s="3">
         <v>11</v>
       </c>
-      <c r="O64" s="8">
-        <f t="shared" si="1"/>
+      <c r="Q64" s="8">
+        <f t="shared" si="2"/>
         <v>0.7857142857142857</v>
       </c>
-      <c r="P64" s="3">
+      <c r="R64" s="3">
         <v>3</v>
       </c>
-      <c r="Q64" s="8">
+      <c r="S64" s="8">
         <v>12.347</v>
       </c>
-      <c r="R64" s="8">
+      <c r="T64" s="8">
         <v>11.71</v>
       </c>
-      <c r="S64" s="8">
+      <c r="U64" s="8">
         <v>11.647</v>
       </c>
-      <c r="T64" s="7">
+      <c r="V64" s="7">
         <v>11.901333333333334</v>
       </c>
     </row>
-    <row r="65" spans="1:20" s="1" customFormat="1">
+    <row r="65" spans="1:22" s="1" customFormat="1">
       <c r="A65" s="3">
         <v>20151017</v>
       </c>
@@ -5456,32 +5908,39 @@
         <v>13</v>
       </c>
       <c r="M65" s="3">
+        <v>17</v>
+      </c>
+      <c r="N65" s="3">
+        <f t="shared" si="1"/>
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="O65" s="3">
         <v>9</v>
       </c>
-      <c r="N65" s="3">
+      <c r="P65" s="3">
         <v>9</v>
       </c>
-      <c r="O65" s="8">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="P65" s="3">
+      <c r="Q65" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="R65" s="3">
         <v>3</v>
       </c>
-      <c r="Q65" s="8">
+      <c r="S65" s="8">
         <v>12.076000000000001</v>
       </c>
-      <c r="R65" s="8">
+      <c r="T65" s="8">
         <v>12.929</v>
       </c>
-      <c r="S65" s="8">
+      <c r="U65" s="8">
         <v>12.073</v>
       </c>
-      <c r="T65" s="7">
+      <c r="V65" s="7">
         <v>12.359333333333334</v>
       </c>
     </row>
-    <row r="66" spans="1:20" s="1" customFormat="1">
+    <row r="66" spans="1:22" s="1" customFormat="1">
       <c r="A66" s="3">
         <v>20151017</v>
       </c>
@@ -5519,32 +5978,39 @@
         <v>20</v>
       </c>
       <c r="M66" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N66" s="3">
-        <v>1</v>
-      </c>
-      <c r="O66" s="8">
-        <f t="shared" ref="O66:O82" si="2">N66/K66</f>
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="O66" s="3">
+        <v>1</v>
+      </c>
+      <c r="P66" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q66" s="8">
+        <f t="shared" ref="Q66:Q82" si="3">P66/K66</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="P66" s="3">
+      <c r="R66" s="3">
         <v>3</v>
       </c>
-      <c r="Q66" s="8">
+      <c r="S66" s="8">
         <v>11.324</v>
       </c>
-      <c r="R66" s="8">
+      <c r="T66" s="8">
         <v>11.763999999999999</v>
       </c>
-      <c r="S66" s="8">
+      <c r="U66" s="8">
         <v>11.157999999999999</v>
       </c>
-      <c r="T66" s="7">
+      <c r="V66" s="7">
         <v>11.415333333333335</v>
       </c>
     </row>
-    <row r="67" spans="1:20" s="1" customFormat="1">
+    <row r="67" spans="1:22" s="1" customFormat="1">
       <c r="A67" s="3">
         <v>20151017</v>
       </c>
@@ -5582,32 +6048,39 @@
         <v>13</v>
       </c>
       <c r="M67" s="3">
+        <v>2</v>
+      </c>
+      <c r="N67" s="3">
+        <f t="shared" ref="N67:N82" si="4">L67/M67</f>
+        <v>6.5</v>
+      </c>
+      <c r="O67" s="3">
         <v>9</v>
       </c>
-      <c r="N67" s="3">
+      <c r="P67" s="3">
         <v>10</v>
       </c>
-      <c r="O67" s="8">
-        <f t="shared" si="2"/>
+      <c r="Q67" s="8">
+        <f t="shared" si="3"/>
         <v>0.76923076923076927</v>
       </c>
-      <c r="P67" s="3">
+      <c r="R67" s="3">
         <v>3</v>
       </c>
-      <c r="Q67" s="8">
+      <c r="S67" s="8">
         <v>11.445</v>
       </c>
-      <c r="R67" s="8">
+      <c r="T67" s="8">
         <v>12.077999999999999</v>
       </c>
-      <c r="S67" s="8">
+      <c r="U67" s="8">
         <v>11.564</v>
       </c>
-      <c r="T67" s="7">
+      <c r="V67" s="7">
         <v>11.695666666666668</v>
       </c>
     </row>
-    <row r="68" spans="1:20" s="1" customFormat="1">
+    <row r="68" spans="1:22" s="1" customFormat="1">
       <c r="A68" s="3">
         <v>20151022</v>
       </c>
@@ -5645,32 +6118,39 @@
         <v>24</v>
       </c>
       <c r="M68" s="3">
+        <v>2</v>
+      </c>
+      <c r="N68" s="3">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="O68" s="3">
         <v>8</v>
       </c>
-      <c r="N68" s="3">
+      <c r="P68" s="3">
         <v>8</v>
       </c>
-      <c r="O68" s="8">
-        <f t="shared" si="2"/>
+      <c r="Q68" s="8">
+        <f t="shared" si="3"/>
         <v>0.5714285714285714</v>
       </c>
-      <c r="P68" s="3">
+      <c r="R68" s="3">
         <v>3</v>
       </c>
-      <c r="Q68" s="9">
+      <c r="S68" s="9">
         <v>11.098000000000001</v>
       </c>
-      <c r="R68" s="9">
+      <c r="T68" s="9">
         <v>11.78</v>
       </c>
-      <c r="S68" s="9">
+      <c r="U68" s="9">
         <v>10.726000000000001</v>
       </c>
-      <c r="T68" s="7">
+      <c r="V68" s="7">
         <v>11.201333333333332</v>
       </c>
     </row>
-    <row r="69" spans="1:20" s="1" customFormat="1">
+    <row r="69" spans="1:22" s="1" customFormat="1">
       <c r="A69" s="3">
         <v>20151022</v>
       </c>
@@ -5708,32 +6188,39 @@
         <v>23</v>
       </c>
       <c r="M69" s="3">
+        <v>17</v>
+      </c>
+      <c r="N69" s="3">
+        <f t="shared" si="4"/>
+        <v>1.3529411764705883</v>
+      </c>
+      <c r="O69" s="3">
         <v>5</v>
       </c>
-      <c r="N69" s="3">
+      <c r="P69" s="3">
         <v>5</v>
       </c>
-      <c r="O69" s="8">
-        <f t="shared" si="2"/>
+      <c r="Q69" s="8">
+        <f t="shared" si="3"/>
         <v>0.41666666666666669</v>
       </c>
-      <c r="P69" s="3" t="s">
+      <c r="R69" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="Q69" s="9">
+      <c r="S69" s="9">
         <v>11.475</v>
       </c>
-      <c r="R69" s="9">
+      <c r="T69" s="9">
         <v>10.986000000000001</v>
       </c>
-      <c r="S69" s="9">
+      <c r="U69" s="9">
         <v>11.898</v>
       </c>
-      <c r="T69" s="7">
+      <c r="V69" s="7">
         <v>11.452999999999998</v>
       </c>
     </row>
-    <row r="70" spans="1:20" s="1" customFormat="1">
+    <row r="70" spans="1:22" s="1" customFormat="1">
       <c r="A70" s="3">
         <v>20151022</v>
       </c>
@@ -5774,29 +6261,36 @@
         <v>2</v>
       </c>
       <c r="N70" s="3">
-        <v>2</v>
-      </c>
-      <c r="O70" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="O70" s="3">
+        <v>2</v>
+      </c>
+      <c r="P70" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q70" s="8">
+        <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="P70" s="3" t="s">
+      <c r="R70" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="Q70" s="9">
+      <c r="S70" s="9">
         <v>11.816000000000001</v>
       </c>
-      <c r="R70" s="9">
+      <c r="T70" s="9">
         <v>12.4</v>
       </c>
-      <c r="S70" s="9">
+      <c r="U70" s="9">
         <v>12.407</v>
       </c>
-      <c r="T70" s="7">
+      <c r="V70" s="7">
         <v>12.207666666666668</v>
       </c>
     </row>
-    <row r="71" spans="1:20" s="1" customFormat="1">
+    <row r="71" spans="1:22" s="1" customFormat="1">
       <c r="A71" s="3">
         <v>20151025</v>
       </c>
@@ -5834,32 +6328,39 @@
         <v>11</v>
       </c>
       <c r="M71" s="3">
+        <v>2</v>
+      </c>
+      <c r="N71" s="3">
+        <f t="shared" si="4"/>
+        <v>5.5</v>
+      </c>
+      <c r="O71" s="3">
         <v>8</v>
       </c>
-      <c r="N71" s="3">
+      <c r="P71" s="3">
         <v>8</v>
       </c>
-      <c r="O71" s="8">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P71" s="3" t="s">
+      <c r="Q71" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R71" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="Q71" s="9">
+      <c r="S71" s="9">
         <v>11.612</v>
       </c>
-      <c r="R71" s="9">
+      <c r="T71" s="9">
         <v>12.048</v>
       </c>
-      <c r="S71" s="9">
+      <c r="U71" s="9">
         <v>11.532</v>
       </c>
-      <c r="T71" s="7">
+      <c r="V71" s="7">
         <v>11.730666666666666</v>
       </c>
     </row>
-    <row r="72" spans="1:20">
+    <row r="72" spans="1:22">
       <c r="A72" s="3">
         <v>20151025</v>
       </c>
@@ -5897,32 +6398,39 @@
         <v>9</v>
       </c>
       <c r="M72" s="3">
+        <v>17</v>
+      </c>
+      <c r="N72" s="3">
+        <f t="shared" si="4"/>
+        <v>0.52941176470588236</v>
+      </c>
+      <c r="O72" s="3">
         <v>6</v>
       </c>
-      <c r="N72" s="3">
+      <c r="P72" s="3">
         <v>7</v>
       </c>
-      <c r="O72" s="8">
-        <f t="shared" si="2"/>
+      <c r="Q72" s="8">
+        <f t="shared" si="3"/>
         <v>0.875</v>
       </c>
-      <c r="P72" s="3">
+      <c r="R72" s="3">
         <v>3</v>
       </c>
-      <c r="Q72" s="9">
+      <c r="S72" s="9">
         <v>11.587</v>
       </c>
-      <c r="R72" s="9">
+      <c r="T72" s="9">
         <v>11.994999999999999</v>
       </c>
-      <c r="S72" s="9">
+      <c r="U72" s="9">
         <v>11.361000000000001</v>
       </c>
-      <c r="T72" s="7">
+      <c r="V72" s="7">
         <v>11.647666666666666</v>
       </c>
     </row>
-    <row r="73" spans="1:20">
+    <row r="73" spans="1:22">
       <c r="A73" s="3">
         <v>20151025</v>
       </c>
@@ -5960,32 +6468,39 @@
         <v>25</v>
       </c>
       <c r="M73" s="3">
+        <v>2</v>
+      </c>
+      <c r="N73" s="3">
+        <f t="shared" si="4"/>
+        <v>12.5</v>
+      </c>
+      <c r="O73" s="3">
         <v>7</v>
       </c>
-      <c r="N73" s="3">
+      <c r="P73" s="3">
         <v>7</v>
       </c>
-      <c r="O73" s="8">
-        <f t="shared" si="2"/>
+      <c r="Q73" s="8">
+        <f t="shared" si="3"/>
         <v>0.63636363636363635</v>
       </c>
-      <c r="P73" s="3">
+      <c r="R73" s="3">
         <v>3</v>
       </c>
-      <c r="Q73" s="9">
+      <c r="S73" s="9">
         <v>11.644</v>
       </c>
-      <c r="R73" s="9">
+      <c r="T73" s="9">
         <v>11.853</v>
       </c>
-      <c r="S73" s="9">
+      <c r="U73" s="9">
         <v>11.542999999999999</v>
       </c>
-      <c r="T73" s="7">
+      <c r="V73" s="7">
         <v>11.68</v>
       </c>
     </row>
-    <row r="74" spans="1:20">
+    <row r="74" spans="1:22">
       <c r="A74" s="3">
         <v>20151026</v>
       </c>
@@ -6023,32 +6538,39 @@
         <v>36</v>
       </c>
       <c r="M74" s="3">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="N74" s="3">
-        <v>2</v>
-      </c>
-      <c r="O74" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
+        <v>2.1176470588235294</v>
+      </c>
+      <c r="O74" s="3">
+        <v>2</v>
+      </c>
+      <c r="P74" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q74" s="8">
+        <f t="shared" si="3"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="P74" s="3">
+      <c r="R74" s="3">
         <v>3</v>
       </c>
-      <c r="Q74" s="9">
+      <c r="S74" s="9">
         <v>12.707000000000001</v>
       </c>
-      <c r="R74" s="9">
+      <c r="T74" s="9">
         <v>12.127000000000001</v>
       </c>
-      <c r="S74" s="9">
+      <c r="U74" s="9">
         <v>12.138999999999999</v>
       </c>
-      <c r="T74" s="7">
+      <c r="V74" s="7">
         <v>12.324333333333334</v>
       </c>
     </row>
-    <row r="75" spans="1:20">
+    <row r="75" spans="1:22">
       <c r="A75" s="3">
         <v>20151026</v>
       </c>
@@ -6086,32 +6608,39 @@
         <v>18</v>
       </c>
       <c r="M75" s="3">
+        <v>2</v>
+      </c>
+      <c r="N75" s="3">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="O75" s="3">
         <v>7</v>
       </c>
-      <c r="N75" s="3">
+      <c r="P75" s="3">
         <v>7</v>
       </c>
-      <c r="O75" s="8">
-        <f t="shared" si="2"/>
+      <c r="Q75" s="8">
+        <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
-      <c r="P75" s="3">
+      <c r="R75" s="3">
         <v>3</v>
       </c>
-      <c r="Q75" s="9">
+      <c r="S75" s="9">
         <v>11.817</v>
       </c>
-      <c r="R75" s="9">
+      <c r="T75" s="9">
         <v>11.654</v>
       </c>
-      <c r="S75" s="9">
+      <c r="U75" s="9">
         <v>11.891</v>
       </c>
-      <c r="T75" s="7">
+      <c r="V75" s="7">
         <v>11.787333333333335</v>
       </c>
     </row>
-    <row r="76" spans="1:20">
+    <row r="76" spans="1:22">
       <c r="A76" s="3">
         <v>20151026</v>
       </c>
@@ -6149,32 +6678,39 @@
         <v>39</v>
       </c>
       <c r="M76" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N76" s="3">
-        <v>1</v>
-      </c>
-      <c r="O76" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
+        <v>19.5</v>
+      </c>
+      <c r="O76" s="3">
+        <v>1</v>
+      </c>
+      <c r="P76" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q76" s="8">
+        <f t="shared" si="3"/>
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="P76" s="3">
+      <c r="R76" s="3">
         <v>3</v>
       </c>
-      <c r="Q76" s="9">
+      <c r="S76" s="9">
         <v>11.968999999999999</v>
       </c>
-      <c r="R76" s="9">
+      <c r="T76" s="9">
         <v>12.178000000000001</v>
       </c>
-      <c r="S76" s="9">
+      <c r="U76" s="9">
         <v>11.683</v>
       </c>
-      <c r="T76" s="7">
+      <c r="V76" s="7">
         <v>11.943333333333333</v>
       </c>
     </row>
-    <row r="77" spans="1:20">
+    <row r="77" spans="1:22">
       <c r="A77" s="3">
         <v>20151026</v>
       </c>
@@ -6212,32 +6748,39 @@
         <v>27</v>
       </c>
       <c r="M77" s="3">
+        <v>2</v>
+      </c>
+      <c r="N77" s="3">
+        <f t="shared" si="4"/>
+        <v>13.5</v>
+      </c>
+      <c r="O77" s="3">
         <v>5</v>
       </c>
-      <c r="N77" s="3">
+      <c r="P77" s="3">
         <v>6</v>
       </c>
-      <c r="O77" s="8">
-        <f t="shared" si="2"/>
+      <c r="Q77" s="8">
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
-      <c r="P77" s="3">
+      <c r="R77" s="3">
         <v>3</v>
       </c>
-      <c r="Q77" s="9">
+      <c r="S77" s="9">
         <v>11.401</v>
       </c>
-      <c r="R77" s="9">
+      <c r="T77" s="9">
         <v>11.8</v>
       </c>
-      <c r="S77" s="9">
+      <c r="U77" s="9">
         <v>11.42</v>
       </c>
-      <c r="T77" s="7">
+      <c r="V77" s="7">
         <v>11.540333333333335</v>
       </c>
     </row>
-    <row r="78" spans="1:20">
+    <row r="78" spans="1:22">
       <c r="A78" s="3">
         <v>20151026</v>
       </c>
@@ -6275,32 +6818,39 @@
         <v>16</v>
       </c>
       <c r="M78" s="3">
+        <v>2</v>
+      </c>
+      <c r="N78" s="3">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="O78" s="3">
         <v>11</v>
       </c>
-      <c r="N78" s="3">
+      <c r="P78" s="3">
         <v>11</v>
       </c>
-      <c r="O78" s="8">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P78" s="3">
+      <c r="Q78" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R78" s="3">
         <v>3</v>
       </c>
-      <c r="Q78" s="9">
+      <c r="S78" s="9">
         <v>11.603</v>
       </c>
-      <c r="R78" s="9">
+      <c r="T78" s="9">
         <v>11.897</v>
       </c>
-      <c r="S78" s="9">
+      <c r="U78" s="9">
         <v>12.335000000000001</v>
       </c>
-      <c r="T78" s="7">
+      <c r="V78" s="7">
         <v>11.945</v>
       </c>
     </row>
-    <row r="79" spans="1:20">
+    <row r="79" spans="1:22">
       <c r="A79" s="3">
         <v>20151026</v>
       </c>
@@ -6338,32 +6888,39 @@
         <v>76</v>
       </c>
       <c r="M79" s="3">
+        <v>17</v>
+      </c>
+      <c r="N79" s="3">
+        <f t="shared" si="4"/>
+        <v>4.4705882352941178</v>
+      </c>
+      <c r="O79" s="3">
         <v>7</v>
       </c>
-      <c r="N79" s="3">
+      <c r="P79" s="3">
         <v>7</v>
       </c>
-      <c r="O79" s="8">
-        <f t="shared" si="2"/>
+      <c r="Q79" s="8">
+        <f t="shared" si="3"/>
         <v>0.63636363636363635</v>
       </c>
-      <c r="P79" s="3" t="s">
+      <c r="R79" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="Q79" s="9">
+      <c r="S79" s="9">
         <v>11.813000000000001</v>
       </c>
-      <c r="R79" s="9">
+      <c r="T79" s="9">
         <v>10.782999999999999</v>
       </c>
-      <c r="S79" s="9">
+      <c r="U79" s="9">
         <v>11.516</v>
       </c>
-      <c r="T79" s="7">
+      <c r="V79" s="7">
         <v>11.370666666666667</v>
       </c>
     </row>
-    <row r="80" spans="1:20">
+    <row r="80" spans="1:22">
       <c r="A80" s="3">
         <v>20151026</v>
       </c>
@@ -6401,32 +6958,39 @@
         <v>18</v>
       </c>
       <c r="M80" s="3">
+        <v>17</v>
+      </c>
+      <c r="N80" s="3">
+        <f t="shared" si="4"/>
+        <v>1.0588235294117647</v>
+      </c>
+      <c r="O80" s="3">
         <v>10</v>
       </c>
-      <c r="N80" s="3">
+      <c r="P80" s="3">
         <v>10</v>
       </c>
-      <c r="O80" s="8">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P80" s="3">
+      <c r="Q80" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R80" s="3">
         <v>3</v>
       </c>
-      <c r="Q80" s="9">
+      <c r="S80" s="9">
         <v>11.308</v>
       </c>
-      <c r="R80" s="9">
+      <c r="T80" s="9">
         <v>10.884</v>
       </c>
-      <c r="S80" s="9">
+      <c r="U80" s="9">
         <v>11.484999999999999</v>
       </c>
-      <c r="T80" s="7">
+      <c r="V80" s="7">
         <v>11.225666666666667</v>
       </c>
     </row>
-    <row r="81" spans="1:20">
+    <row r="81" spans="1:22">
       <c r="A81" s="3">
         <v>20151026</v>
       </c>
@@ -6464,32 +7028,39 @@
         <v>26</v>
       </c>
       <c r="M81" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N81" s="3">
-        <v>2</v>
-      </c>
-      <c r="O81" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="O81" s="3">
+        <v>1</v>
+      </c>
+      <c r="P81" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q81" s="8">
+        <f t="shared" si="3"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="P81" s="3">
+      <c r="R81" s="3">
         <v>3</v>
       </c>
-      <c r="Q81" s="9">
+      <c r="S81" s="9">
         <v>12.154</v>
       </c>
-      <c r="R81" s="9">
+      <c r="T81" s="9">
         <v>11.631</v>
       </c>
-      <c r="S81" s="9">
+      <c r="U81" s="9">
         <v>11.849</v>
       </c>
-      <c r="T81" s="7">
+      <c r="V81" s="7">
         <v>11.878</v>
       </c>
     </row>
-    <row r="82" spans="1:20">
+    <row r="82" spans="1:22">
       <c r="A82" s="3">
         <v>20151026</v>
       </c>
@@ -6527,184 +7098,37 @@
         <v>11</v>
       </c>
       <c r="M82" s="3">
+        <v>2</v>
+      </c>
+      <c r="N82" s="3">
+        <f t="shared" si="4"/>
+        <v>5.5</v>
+      </c>
+      <c r="O82" s="3">
         <v>7</v>
       </c>
-      <c r="N82" s="3">
+      <c r="P82" s="3">
         <v>7</v>
       </c>
-      <c r="O82" s="8">
-        <f t="shared" si="2"/>
+      <c r="Q82" s="8">
+        <f t="shared" si="3"/>
         <v>0.77777777777777779</v>
       </c>
-      <c r="P82" s="3">
+      <c r="R82" s="3">
         <v>3</v>
       </c>
-      <c r="Q82" s="9">
+      <c r="S82" s="9">
         <v>11.56</v>
       </c>
-      <c r="R82" s="9">
+      <c r="T82" s="9">
         <v>11.377000000000001</v>
       </c>
-      <c r="S82" s="9">
+      <c r="U82" s="9">
         <v>11.778</v>
       </c>
-      <c r="T82" s="7">
+      <c r="V82" s="7">
         <v>11.571666666666667</v>
       </c>
-    </row>
-    <row r="84" spans="1:20">
-      <c r="A84"/>
-      <c r="B84"/>
-      <c r="C84"/>
-      <c r="D84"/>
-      <c r="E84"/>
-      <c r="F84"/>
-      <c r="G84"/>
-      <c r="H84"/>
-      <c r="I84"/>
-      <c r="J84"/>
-      <c r="K84"/>
-      <c r="L84"/>
-      <c r="M84"/>
-      <c r="N84"/>
-      <c r="O84"/>
-      <c r="P84"/>
-      <c r="Q84"/>
-      <c r="R84"/>
-      <c r="S84"/>
-      <c r="T84"/>
-    </row>
-    <row r="85" spans="1:20">
-      <c r="A85"/>
-      <c r="B85"/>
-      <c r="C85"/>
-      <c r="D85"/>
-      <c r="E85"/>
-      <c r="F85"/>
-      <c r="G85"/>
-      <c r="H85"/>
-      <c r="I85"/>
-      <c r="J85"/>
-      <c r="K85"/>
-      <c r="L85"/>
-      <c r="M85"/>
-      <c r="N85"/>
-      <c r="O85"/>
-      <c r="P85"/>
-      <c r="Q85"/>
-      <c r="R85"/>
-      <c r="S85"/>
-      <c r="T85"/>
-    </row>
-    <row r="86" spans="1:20">
-      <c r="A86"/>
-      <c r="B86"/>
-      <c r="C86"/>
-      <c r="D86"/>
-      <c r="E86"/>
-      <c r="F86"/>
-      <c r="G86"/>
-      <c r="H86"/>
-      <c r="I86"/>
-      <c r="J86"/>
-      <c r="K86"/>
-      <c r="L86"/>
-      <c r="M86"/>
-      <c r="N86"/>
-      <c r="O86"/>
-      <c r="P86"/>
-      <c r="Q86"/>
-      <c r="R86"/>
-      <c r="S86"/>
-      <c r="T86"/>
-    </row>
-    <row r="87" spans="1:20">
-      <c r="A87"/>
-      <c r="B87"/>
-      <c r="C87"/>
-      <c r="D87"/>
-      <c r="E87"/>
-      <c r="F87"/>
-      <c r="G87"/>
-      <c r="H87"/>
-      <c r="I87"/>
-      <c r="J87"/>
-      <c r="K87"/>
-      <c r="L87"/>
-      <c r="M87"/>
-      <c r="N87"/>
-      <c r="O87"/>
-      <c r="P87"/>
-      <c r="Q87"/>
-      <c r="R87"/>
-      <c r="S87"/>
-      <c r="T87"/>
-    </row>
-    <row r="88" spans="1:20">
-      <c r="A88"/>
-      <c r="B88"/>
-      <c r="C88"/>
-      <c r="D88"/>
-      <c r="E88"/>
-      <c r="F88"/>
-      <c r="G88"/>
-      <c r="H88"/>
-      <c r="I88"/>
-      <c r="J88"/>
-      <c r="K88"/>
-      <c r="L88"/>
-      <c r="M88"/>
-      <c r="N88"/>
-      <c r="O88"/>
-      <c r="P88"/>
-      <c r="Q88"/>
-      <c r="R88"/>
-      <c r="S88"/>
-      <c r="T88"/>
-    </row>
-    <row r="89" spans="1:20">
-      <c r="A89"/>
-      <c r="B89"/>
-      <c r="C89"/>
-      <c r="D89"/>
-      <c r="E89"/>
-      <c r="F89"/>
-      <c r="G89"/>
-      <c r="H89"/>
-      <c r="I89"/>
-      <c r="J89"/>
-      <c r="K89"/>
-      <c r="L89"/>
-      <c r="M89"/>
-      <c r="N89"/>
-      <c r="O89"/>
-      <c r="P89"/>
-      <c r="Q89"/>
-      <c r="R89"/>
-      <c r="S89"/>
-      <c r="T89"/>
-    </row>
-    <row r="90" spans="1:20">
-      <c r="A90"/>
-      <c r="B90"/>
-      <c r="C90"/>
-      <c r="D90"/>
-      <c r="E90"/>
-      <c r="F90"/>
-      <c r="G90"/>
-      <c r="H90"/>
-      <c r="I90"/>
-      <c r="J90"/>
-      <c r="K90"/>
-      <c r="L90"/>
-      <c r="M90"/>
-      <c r="N90"/>
-      <c r="O90"/>
-      <c r="P90"/>
-      <c r="Q90"/>
-      <c r="R90"/>
-      <c r="S90"/>
-      <c r="T90"/>
     </row>
   </sheetData>
   <sortState ref="A2:R85">

</xml_diff>